<commit_message>
Minor Edits to Excel Sheet
Minor edits to excel sheet.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AED4DC2-7869-4D48-9EDD-061A878BC742}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB435DD3-0242-49F2-835F-03D96BD6099F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="138">
   <si>
     <t>Field name</t>
   </si>
@@ -423,9 +423,6 @@
     <t xml:space="preserve">This denotes any other metadata to be associated with the slice. This will likely be a work in progress. </t>
   </si>
   <si>
-    <t xml:space="preserve">Denotes the type of slice being referenced. Meta data tags may be associated with each type to give supplementary information about the type. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Denotes the width in meters of the slice. </t>
   </si>
   <si>
@@ -433,6 +430,12 @@
   </si>
   <si>
     <t xml:space="preserve">Denotes whether the slice is facing forward (towards the geometry end point) or reverse (towards the geometry start point). </t>
+  </si>
+  <si>
+    <t>Denotes the type of slice being referenced. Meta data tags may be associated with each type to give supplementary information about the type. Type information should correspond to the additive specification, but also provide flexibility for new or emerging lane types.</t>
+  </si>
+  <si>
+    <t>Possible Values</t>
   </si>
 </sst>
 </file>
@@ -776,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1479,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CE16D9-6B4A-4B97-84C9-4C29085A06C3}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1493,14 +1496,15 @@
     <col min="4" max="4" width="20.89453125" customWidth="1"/>
     <col min="5" max="5" width="26.83984375" customWidth="1"/>
     <col min="6" max="6" width="52.05078125" customWidth="1"/>
+    <col min="7" max="7" width="46.9453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" ht="22.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1519,8 +1523,11 @@
       <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>115</v>
       </c>
@@ -1538,7 +1545,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>120</v>
       </c>
@@ -1556,7 +1563,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>122</v>
       </c>
@@ -1574,7 +1581,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>125</v>
@@ -1589,10 +1596,10 @@
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>126</v>
@@ -1607,10 +1614,10 @@
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>127</v>
@@ -1625,10 +1632,10 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>128</v>
@@ -1643,10 +1650,10 @@
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="2" t="s">
         <v>131</v>
       </c>

</xml_diff>

<commit_message>
add draft slice types
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B721FB9B-3A1D-44D1-9FCF-EF40E2A9A2E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC2D4BA-296E-45D6-86E1-0599901B3E00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1010" windowWidth="30050" windowHeight="17810" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="224">
   <si>
     <t>Field name</t>
   </si>
@@ -495,12 +495,249 @@
   <si>
     <t xml:space="preserve">This denotes a through-lane intended for automobile traffic. </t>
   </si>
+  <si>
+    <t>(all)</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>paving</t>
+  </si>
+  <si>
+    <t>Meta tags permitted on all slices</t>
+  </si>
+  <si>
+    <t>A string value indicating painted color for the slice (e.g. "red" is common for bus lanes, "green" or "blue" for bike lanes). Allow some other descriptive words for special patterns or artwork</t>
+  </si>
+  <si>
+    <t>curb_height</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>A string value indicating the paving material of the surface, e.g. "asphalt", "concrete", "cobblestone", "dirt", etc. (There should be some attempt at standardizing common values but allow custom values to be used.) This should not be a required value because specific slices can assume default values, e.g. the default value of paving for a drive_lane, if not specified, is "asphalt". Allow "none" if slice is not paved; e.g. plants, water</t>
+  </si>
+  <si>
+    <t>A relative number for the height of the surface. Rather than deal with specific measurements (which can vary depending on elevation and other factors) we (that is, Streetmix) uses 0 to indicate a road surface and 1 for a raised sidewalk surface. If there is no height difference between the drive_lane and sidewalk areas, the values will both be 0. A surface at half-curb-height is 0.5. Ditches are given negative values. Raised platforms can be given any number above 1 that represents a relative scale factor compared to the difference in height between the sidewalk curb and road surface (e.g. 2, 2.5, 3, etc)</t>
+  </si>
+  <si>
+    <t>bike_lane</t>
+  </si>
+  <si>
+    <t>sidewalk</t>
+  </si>
+  <si>
+    <t>transitions</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Not entirely sure how this should be defined, but this property describes how the edge of one slice should transition to a neighboring slice based on some criteria. E.g. a drive_lane next to another_drive lane might have a transition of a broken white line. A raised curb next to an asphant-paved slice might have a gutter, or a ramp, or other types of transitions.</t>
+  </si>
+  <si>
+    <t>turn_lane</t>
+  </si>
+  <si>
+    <t>limitless</t>
+  </si>
+  <si>
+    <t>bus_lane</t>
+  </si>
+  <si>
+    <t>brt</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>transit</t>
+  </si>
+  <si>
+    <t>Whether the bus lane allows bikes (may have a sharrow stamp)</t>
+  </si>
+  <si>
+    <t>bikes_allowed</t>
+  </si>
+  <si>
+    <t>taxi_allowed</t>
+  </si>
+  <si>
+    <t>Whether the bus lane allows taxis (or other shared mobility)</t>
+  </si>
+  <si>
+    <t>parklet</t>
+  </si>
+  <si>
+    <t>VERY ROUGH DRAFT!</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>buffer</t>
+  </si>
+  <si>
+    <t>temporary</t>
+  </si>
+  <si>
+    <t>A lane where automobiles are taken out of traffic flow in order to queue for turning</t>
+  </si>
+  <si>
+    <t>A turn_lane may have a sharrow stamp</t>
+  </si>
+  <si>
+    <t>NON-AUTOMOTIVE (DEDICATED)</t>
+  </si>
+  <si>
+    <t>AUTOMOTIVE (DEDICATED)</t>
+  </si>
+  <si>
+    <t>CURB ZONE</t>
+  </si>
+  <si>
+    <t>MIXED LANES</t>
+  </si>
+  <si>
+    <t>MISCELLANEOUS</t>
+  </si>
+  <si>
+    <t>Through-lane dedicated to busses.</t>
+  </si>
+  <si>
+    <t>Through-lane dedicated to bicycles or other vehicles of similar shape and speed.</t>
+  </si>
+  <si>
+    <t>Through-lane dedicated to pedestrians, usually (but not always) on a raised curb</t>
+  </si>
+  <si>
+    <t>"Dedicated" means "primarily intended for." In each of these cases mixed traffic may be permitted and a meta tag will indicate what kind of mixing is allowed.</t>
+  </si>
+  <si>
+    <t>accessible</t>
+  </si>
+  <si>
+    <t>Sidewalk meets accessibility regulations (e.g. ADA in the US)</t>
+  </si>
+  <si>
+    <t>Whether the bus lane is dedicated to bus rapid transit as opposed to regular buses.</t>
+  </si>
+  <si>
+    <t>A through-lane with fixed infrastructure (e.g. rail-based transit)</t>
+  </si>
+  <si>
+    <t>A string value indicating the type of rail transit (trolley, light rail, heavy rail)</t>
+  </si>
+  <si>
+    <t>Whether the transit lane permits automobiles.</t>
+  </si>
+  <si>
+    <t>autos_allowed</t>
+  </si>
+  <si>
+    <t>bus_allowed</t>
+  </si>
+  <si>
+    <t>Whether the transit lane permits non-fixed-rail transit, e.g. buses</t>
+  </si>
+  <si>
+    <t>see above</t>
+  </si>
+  <si>
+    <t>A specially designated through-lane intended for any non-automotive vehicle.</t>
+  </si>
+  <si>
+    <t>flex_zone</t>
+  </si>
+  <si>
+    <t>A lane dedicated for automobile parking.</t>
+  </si>
+  <si>
+    <t>A parking area converted to a pedestrian-use area.</t>
+  </si>
+  <si>
+    <t>Generic designation for a curb zone with varying uses.</t>
+  </si>
+  <si>
+    <t>freight_loading</t>
+  </si>
+  <si>
+    <t>passenger_loading</t>
+  </si>
+  <si>
+    <t>A loading zone, primarily for passenger pickup/dropoff.</t>
+  </si>
+  <si>
+    <t>A loading zone, primarily for the loading and unloading of goods</t>
+  </si>
+  <si>
+    <t>Any slice that has been reconfigured for a temporary purpose, e.g construction</t>
+  </si>
+  <si>
+    <t>barrier_type</t>
+  </si>
+  <si>
+    <t>If the slice is a barrier, type of barrier (e.g. traffic cone, jersey barrier, fencing, etc)</t>
+  </si>
+  <si>
+    <t>What is this temporary purpose (e.g. construction, event)</t>
+  </si>
+  <si>
+    <t>commercial</t>
+  </si>
+  <si>
+    <t>A zone where commerce is permitted, e.g. food trucks, farmer's markets, newstands</t>
+  </si>
+  <si>
+    <t>transit_shelter</t>
+  </si>
+  <si>
+    <t>An area / platform for waiting for transit</t>
+  </si>
+  <si>
+    <t>auto_parking</t>
+  </si>
+  <si>
+    <t>bike_parking</t>
+  </si>
+  <si>
+    <t>bike_share</t>
+  </si>
+  <si>
+    <t>scooter_parking</t>
+  </si>
+  <si>
+    <t>planting_strip</t>
+  </si>
+  <si>
+    <t>canal</t>
+  </si>
+  <si>
+    <t>A water channel</t>
+  </si>
+  <si>
+    <t>An area for plants, primarily for decorative purposes (though it can have an ecological impact). Usually placed in a sidewalk (as opposed to a median) This differentiates this from:</t>
+  </si>
+  <si>
+    <t>filter_strip</t>
+  </si>
+  <si>
+    <t>An area designated for stormwater management, which is usually (but not required to be) vegetated.</t>
+  </si>
+  <si>
+    <t>Curb zones are the liminal space between through traffic and a pedestrian zone which have usually been reserved for automobile parking, but more recently, segments of the curb zone have been chopped up and designated for other uses. Therefore curb zones may be portions of slices from point A to B. Note that there is a very fine line between some types of uses in a curb zone and miscellaneous objects.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,6 +761,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -555,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -563,6 +813,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,20 +1110,20 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="32.83984375" customWidth="1"/>
-    <col min="3" max="3" width="20.9453125" customWidth="1"/>
-    <col min="4" max="4" width="18.3125" customWidth="1"/>
-    <col min="5" max="5" width="77.20703125" customWidth="1"/>
+    <col min="1" max="2" width="32.81640625" customWidth="1"/>
+    <col min="3" max="3" width="20.90625" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" customWidth="1"/>
+    <col min="5" max="5" width="77.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -879,7 +1140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -896,7 +1157,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>117</v>
       </c>
@@ -913,7 +1174,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -930,7 +1191,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -947,7 +1208,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -964,7 +1225,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -981,7 +1242,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -998,7 +1259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1015,7 +1276,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -1032,7 +1293,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -1049,7 +1310,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
@@ -1066,7 +1327,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
@@ -1083,7 +1344,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
@@ -1100,7 +1361,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -1117,7 +1378,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>35</v>
       </c>
@@ -1134,7 +1395,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
@@ -1151,7 +1412,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1168,7 +1429,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1185,7 +1446,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -1202,7 +1463,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>71</v>
       </c>
@@ -1219,7 +1480,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>73</v>
       </c>
@@ -1236,7 +1497,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
@@ -1253,7 +1514,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>75</v>
       </c>
@@ -1270,7 +1531,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>77</v>
       </c>
@@ -1287,7 +1548,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>79</v>
       </c>
@@ -1304,7 +1565,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>81</v>
       </c>
@@ -1321,7 +1582,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>83</v>
       </c>
@@ -1338,7 +1599,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>85</v>
       </c>
@@ -1355,7 +1616,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>87</v>
       </c>
@@ -1372,7 +1633,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>89</v>
       </c>
@@ -1389,7 +1650,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>90</v>
       </c>
@@ -1406,7 +1667,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>92</v>
       </c>
@@ -1423,7 +1684,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>93</v>
       </c>
@@ -1440,7 +1701,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>95</v>
       </c>
@@ -1457,7 +1718,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -1474,7 +1735,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -1491,7 +1752,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -1508,7 +1769,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -1540,7 +1801,7 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1554,22 +1815,22 @@
       <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.734375" customWidth="1"/>
-    <col min="2" max="2" width="11.7890625" customWidth="1"/>
-    <col min="3" max="3" width="33.89453125" customWidth="1"/>
-    <col min="4" max="4" width="20.89453125" customWidth="1"/>
-    <col min="5" max="5" width="26.83984375" customWidth="1"/>
-    <col min="6" max="6" width="52.05078125" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="33.90625" customWidth="1"/>
+    <col min="4" max="4" width="20.90625" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" customWidth="1"/>
+    <col min="6" max="6" width="52.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1589,7 +1850,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>115</v>
       </c>
@@ -1607,7 +1868,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>120</v>
       </c>
@@ -1625,7 +1886,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>122</v>
       </c>
@@ -1643,7 +1904,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>125</v>
@@ -1661,7 +1922,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>126</v>
@@ -1679,7 +1940,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>127</v>
@@ -1697,7 +1958,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
         <v>128</v>
@@ -1715,7 +1976,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>131</v>
       </c>
@@ -1740,26 +2001,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14113956-9C41-4528-BBB9-AD2809B184AF}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.3671875" customWidth="1"/>
-    <col min="3" max="3" width="30.1015625" customWidth="1"/>
-    <col min="4" max="4" width="28.15625" customWidth="1"/>
-    <col min="5" max="5" width="76.05078125" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" customWidth="1"/>
+    <col min="2" max="2" width="20.36328125" customWidth="1"/>
+    <col min="3" max="3" width="30.08984375" customWidth="1"/>
+    <col min="4" max="4" width="28.1796875" customWidth="1"/>
+    <col min="5" max="5" width="76.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>138</v>
       </c>
@@ -1776,35 +2043,477 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>140</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C12" t="s">
         <v>129</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D12" t="s">
         <v>142</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E12" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
         <v>141</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>186</v>
+      </c>
+      <c r="C18" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>168</v>
+      </c>
+      <c r="C23" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" t="s">
         <v>129</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>192</v>
+      </c>
+      <c r="C26" t="s">
+        <v>164</v>
+      </c>
+      <c r="D26" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>143</v>
-      </c>
+      <c r="E26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>193</v>
+      </c>
+      <c r="C27" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" t="s">
+        <v>164</v>
+      </c>
+      <c r="D28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>161</v>
+      </c>
+      <c r="E32" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>197</v>
+      </c>
+      <c r="E35" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>213</v>
+      </c>
+      <c r="E36" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>170</v>
+      </c>
+      <c r="E37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>201</v>
+      </c>
+      <c r="E38" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>202</v>
+      </c>
+      <c r="E39" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E40" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>174</v>
+      </c>
+      <c r="E50" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>125</v>
+      </c>
+      <c r="E51" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B52" t="s">
+        <v>206</v>
+      </c>
+      <c r="E52" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>211</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>217</v>
+      </c>
+      <c r="E54" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>221</v>
+      </c>
+      <c r="E55" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>218</v>
+      </c>
+      <c r="E56" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Spec with Draft of Slice Types
The following edits were based on review and sheet exchange between
@louh  and @d-wasserman. @louh  made the bulk of these edits,
@d-wasserman  clarified text, reviewed, and made some edits.

@louh the major edit I made was trying to take on the transitions, but I
think you are right this is the hardest aspect to define.

Rought draft on slice space. More edits to come.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B721FB9B-3A1D-44D1-9FCF-EF40E2A9A2E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{472B9B76-4B00-46A5-9E9E-867015977571}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="235">
   <si>
     <t>Field name</t>
   </si>
@@ -495,12 +495,282 @@
   <si>
     <t xml:space="preserve">This denotes a through-lane intended for automobile traffic. </t>
   </si>
+  <si>
+    <t>(all)</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>paving</t>
+  </si>
+  <si>
+    <t>Meta tags permitted on all slices</t>
+  </si>
+  <si>
+    <t>A string value indicating painted color for the slice (e.g. "red" is common for bus lanes, "green" or "blue" for bike lanes). Allow some other descriptive words for special patterns or artwork</t>
+  </si>
+  <si>
+    <t>curb_height</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>A string value indicating the paving material of the surface, e.g. "asphalt", "concrete", "cobblestone", "dirt", etc. (There should be some attempt at standardizing common values but allow custom values to be used.) This should not be a required value because specific slices can assume default values, e.g. the default value of paving for a drive_lane, if not specified, is "asphalt". Allow "none" if slice is not paved; e.g. plants, water</t>
+  </si>
+  <si>
+    <t>A relative number for the height of the surface. Rather than deal with specific measurements (which can vary depending on elevation and other factors) we (that is, Streetmix) uses 0 to indicate a road surface and 1 for a raised sidewalk surface. If there is no height difference between the drive_lane and sidewalk areas, the values will both be 0. A surface at half-curb-height is 0.5. Ditches are given negative values. Raised platforms can be given any number above 1 that represents a relative scale factor compared to the difference in height between the sidewalk curb and road surface (e.g. 2, 2.5, 3, etc)</t>
+  </si>
+  <si>
+    <t>bike_lane</t>
+  </si>
+  <si>
+    <t>sidewalk</t>
+  </si>
+  <si>
+    <t>transitions</t>
+  </si>
+  <si>
+    <t>turn_lane</t>
+  </si>
+  <si>
+    <t>limitless</t>
+  </si>
+  <si>
+    <t>bus_lane</t>
+  </si>
+  <si>
+    <t>brt</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>transit</t>
+  </si>
+  <si>
+    <t>Whether the bus lane allows bikes (may have a sharrow stamp)</t>
+  </si>
+  <si>
+    <t>bikes_allowed</t>
+  </si>
+  <si>
+    <t>taxi_allowed</t>
+  </si>
+  <si>
+    <t>Whether the bus lane allows taxis (or other shared mobility)</t>
+  </si>
+  <si>
+    <t>parklet</t>
+  </si>
+  <si>
+    <t>VERY ROUGH DRAFT!</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>buffer</t>
+  </si>
+  <si>
+    <t>temporary</t>
+  </si>
+  <si>
+    <t>A lane where automobiles are taken out of traffic flow in order to queue for turning</t>
+  </si>
+  <si>
+    <t>A turn_lane may have a sharrow stamp</t>
+  </si>
+  <si>
+    <t>NON-AUTOMOTIVE (DEDICATED)</t>
+  </si>
+  <si>
+    <t>AUTOMOTIVE (DEDICATED)</t>
+  </si>
+  <si>
+    <t>CURB ZONE</t>
+  </si>
+  <si>
+    <t>MIXED LANES</t>
+  </si>
+  <si>
+    <t>MISCELLANEOUS</t>
+  </si>
+  <si>
+    <t>Through-lane dedicated to busses.</t>
+  </si>
+  <si>
+    <t>Through-lane dedicated to bicycles or other vehicles of similar shape and speed.</t>
+  </si>
+  <si>
+    <t>Through-lane dedicated to pedestrians, usually (but not always) on a raised curb</t>
+  </si>
+  <si>
+    <t>"Dedicated" means "primarily intended for." In each of these cases mixed traffic may be permitted and a meta tag will indicate what kind of mixing is allowed.</t>
+  </si>
+  <si>
+    <t>accessible</t>
+  </si>
+  <si>
+    <t>Sidewalk meets accessibility regulations (e.g. ADA in the US)</t>
+  </si>
+  <si>
+    <t>Whether the bus lane is dedicated to bus rapid transit as opposed to regular buses.</t>
+  </si>
+  <si>
+    <t>A through-lane with fixed infrastructure (e.g. rail-based transit)</t>
+  </si>
+  <si>
+    <t>A string value indicating the type of rail transit (trolley, light rail, heavy rail)</t>
+  </si>
+  <si>
+    <t>Whether the transit lane permits automobiles.</t>
+  </si>
+  <si>
+    <t>autos_allowed</t>
+  </si>
+  <si>
+    <t>bus_allowed</t>
+  </si>
+  <si>
+    <t>Whether the transit lane permits non-fixed-rail transit, e.g. buses</t>
+  </si>
+  <si>
+    <t>see above</t>
+  </si>
+  <si>
+    <t>A specially designated through-lane intended for any non-automotive vehicle.</t>
+  </si>
+  <si>
+    <t>flex_zone</t>
+  </si>
+  <si>
+    <t>A lane dedicated for automobile parking.</t>
+  </si>
+  <si>
+    <t>A parking area converted to a pedestrian-use area.</t>
+  </si>
+  <si>
+    <t>Generic designation for a curb zone with varying uses.</t>
+  </si>
+  <si>
+    <t>freight_loading</t>
+  </si>
+  <si>
+    <t>passenger_loading</t>
+  </si>
+  <si>
+    <t>A loading zone, primarily for passenger pickup/dropoff.</t>
+  </si>
+  <si>
+    <t>A loading zone, primarily for the loading and unloading of goods</t>
+  </si>
+  <si>
+    <t>Any slice that has been reconfigured for a temporary purpose, e.g construction</t>
+  </si>
+  <si>
+    <t>barrier_type</t>
+  </si>
+  <si>
+    <t>If the slice is a barrier, type of barrier (e.g. traffic cone, jersey barrier, fencing, etc)</t>
+  </si>
+  <si>
+    <t>What is this temporary purpose (e.g. construction, event)</t>
+  </si>
+  <si>
+    <t>commercial</t>
+  </si>
+  <si>
+    <t>A zone where commerce is permitted, e.g. food trucks, farmer's markets, newstands</t>
+  </si>
+  <si>
+    <t>transit_shelter</t>
+  </si>
+  <si>
+    <t>An area / platform for waiting for transit</t>
+  </si>
+  <si>
+    <t>auto_parking</t>
+  </si>
+  <si>
+    <t>bike_parking</t>
+  </si>
+  <si>
+    <t>bike_share</t>
+  </si>
+  <si>
+    <t>planting_strip</t>
+  </si>
+  <si>
+    <t>canal</t>
+  </si>
+  <si>
+    <t>A water channel</t>
+  </si>
+  <si>
+    <t>An area for plants, primarily for decorative purposes (though it can have an ecological impact). Usually placed in a sidewalk (as opposed to a median) This differentiates this from:</t>
+  </si>
+  <si>
+    <t>filter_strip</t>
+  </si>
+  <si>
+    <t>An area designated for stormwater management, which is usually (but not required to be) vegetated.</t>
+  </si>
+  <si>
+    <t>Curb zones are the liminal space between through traffic and a pedestrian zone which have usually been reserved for automobile parking, but more recently, segments of the curb zone have been chopped up and designated for other uses. Therefore curb zones may be portions of slices from point A to B. Note that there is a very fine line between some types of uses in a curb zone and miscellaneous objects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A zone where some designated of bicycle parking will be placed. </t>
+  </si>
+  <si>
+    <t>dockless_parking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A zone where a docked bicycle share installation will be placed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A zone where dockless bicycle shared or scooters can be parked. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of median allowed. Possible values include: cement, vegetated, vegetated with trees, stone, brick, other. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A raised street slice whose elements  are in the center of the street. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A raised street slice whose elements typically provide some degree of protection to a multimodal lane such as a bike lane. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of buffer allowed. Possible values include: cement, vegetated, vegetated with trees, stone, brick, other. </t>
+  </si>
+  <si>
+    <t>Definition in flux, but these transition properties describe how the edge of one slice should transition to a neighboring slice based on some criteria. E.g. a drive_lane next to another_drive lane might have a transition of a broken white line. A raised curb next to an asphant-paved slice might have a gutter, or a ramp, or other types of transitions.</t>
+  </si>
+  <si>
+    <t>Sub-Meta Tags</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This denotes how end point transitions are defined in the specification. They are in the form: {index_position_of_connecting_street_slice: transition_type}. The index position indicates where the connecting slice is on the other street, and the transition type can have the values of : angled, s-shaped, offset, and semi-circle. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This denotes how start point transitions are defined in the specification. They are in the form: {index_position_of_connecting_street_slice: transition_type}. The index position indicates where the connecting slice is on the other street, and the transition type can have the values of : angled, s-shaped, offset, and semi-circle. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,6 +794,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -555,13 +838,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -845,16 +1145,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="32.83984375" customWidth="1"/>
-    <col min="3" max="3" width="20.9453125" customWidth="1"/>
-    <col min="4" max="4" width="18.3125" customWidth="1"/>
-    <col min="5" max="5" width="77.20703125" customWidth="1"/>
+    <col min="1" max="2" width="32.7890625" customWidth="1"/>
+    <col min="3" max="3" width="20.89453125" customWidth="1"/>
+    <col min="4" max="4" width="18.26171875" customWidth="1"/>
+    <col min="5" max="5" width="77.15625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1550,7 +1850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CE16D9-6B4A-4B97-84C9-4C29085A06C3}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:F5"/>
     </sheetView>
   </sheetViews>
@@ -1560,8 +1860,8 @@
     <col min="2" max="2" width="11.7890625" customWidth="1"/>
     <col min="3" max="3" width="33.89453125" customWidth="1"/>
     <col min="4" max="4" width="20.89453125" customWidth="1"/>
-    <col min="5" max="5" width="26.83984375" customWidth="1"/>
-    <col min="6" max="6" width="52.05078125" customWidth="1"/>
+    <col min="5" max="5" width="26.7890625" customWidth="1"/>
+    <col min="6" max="6" width="52.1015625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1740,26 +2040,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14113956-9C41-4528-BBB9-AD2809B184AF}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="20.3671875" customWidth="1"/>
-    <col min="3" max="3" width="30.1015625" customWidth="1"/>
-    <col min="4" max="4" width="28.15625" customWidth="1"/>
-    <col min="5" max="5" width="76.05078125" customWidth="1"/>
+    <col min="1" max="1" width="15.89453125" customWidth="1"/>
+    <col min="2" max="3" width="20.3671875" customWidth="1"/>
+    <col min="4" max="4" width="30.1015625" customWidth="1"/>
+    <col min="5" max="5" width="28.15625" customWidth="1"/>
+    <col min="6" max="6" width="76.1015625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>138</v>
       </c>
@@ -1767,44 +2073,597 @@
         <v>139</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
         <v>140</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D14" t="s">
         <v>129</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E14" t="s">
         <v>142</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" t="s">
         <v>141</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D15" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F19" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D20" t="s">
+        <v>162</v>
+      </c>
+      <c r="F20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>160</v>
+      </c>
+      <c r="F22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" t="s">
+        <v>161</v>
+      </c>
+      <c r="D23" t="s">
+        <v>162</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>163</v>
+      </c>
+      <c r="F26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" t="s">
         <v>129</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>143</v>
-      </c>
+      <c r="F28" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B30" t="s">
+        <v>165</v>
+      </c>
+      <c r="D30" t="s">
+        <v>162</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" t="s">
+        <v>166</v>
+      </c>
+      <c r="D31" t="s">
+        <v>162</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>159</v>
+      </c>
+      <c r="F34" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>195</v>
+      </c>
+      <c r="E37" t="s">
+        <v>147</v>
+      </c>
+      <c r="F37" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>211</v>
+      </c>
+      <c r="E38" t="s">
+        <v>147</v>
+      </c>
+      <c r="F38" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" t="s">
+        <v>147</v>
+      </c>
+      <c r="F40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>200</v>
+      </c>
+      <c r="E41" t="s">
+        <v>147</v>
+      </c>
+      <c r="F41" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>207</v>
+      </c>
+      <c r="E42" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>212</v>
+      </c>
+      <c r="E43" t="s">
+        <v>147</v>
+      </c>
+      <c r="F43" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>213</v>
+      </c>
+      <c r="E44" t="s">
+        <v>147</v>
+      </c>
+      <c r="F44" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>222</v>
+      </c>
+      <c r="E45" t="s">
+        <v>147</v>
+      </c>
+      <c r="F45" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>170</v>
+      </c>
+      <c r="E48" t="s">
+        <v>142</v>
+      </c>
+      <c r="F48" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B49" t="s">
+        <v>125</v>
+      </c>
+      <c r="F49" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>171</v>
+      </c>
+      <c r="E50" t="s">
+        <v>147</v>
+      </c>
+      <c r="F50" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B51" t="s">
+        <v>125</v>
+      </c>
+      <c r="F51" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" t="s">
+        <v>147</v>
+      </c>
+      <c r="F52" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+      <c r="F53" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" t="s">
+        <v>204</v>
+      </c>
+      <c r="F54" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>209</v>
+      </c>
+      <c r="E55" t="s">
+        <v>147</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>214</v>
+      </c>
+      <c r="E56" t="s">
+        <v>147</v>
+      </c>
+      <c r="F56" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>218</v>
+      </c>
+      <c r="E57" t="s">
+        <v>147</v>
+      </c>
+      <c r="F57" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>215</v>
+      </c>
+      <c r="E58" t="s">
+        <v>147</v>
+      </c>
+      <c r="F58" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A18:B18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add description to crosswalk sheet
Elaborate on other elements, begin the definition of a crosswalk feature
class that can be edited in a SQL/GIS database. It seems like something
that could be built & edited soon.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{472B9B76-4B00-46A5-9E9E-867015977571}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5225A954-22A2-4055-8707-22B28F1B6FC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
-    <sheet name="Crosswalk (In Progress)" sheetId="3" r:id="rId2"/>
+    <sheet name="Crosswalk" sheetId="3" r:id="rId2"/>
     <sheet name="Slice Cross-section Spec" sheetId="2" r:id="rId3"/>
     <sheet name="Slice Types" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="242">
   <si>
     <t>Field name</t>
   </si>
@@ -386,9 +386,6 @@
   </si>
   <si>
     <t>sharedstreetid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SharedStreets ID for the specific segment of interest. This should be a unique ID. </t>
   </si>
   <si>
     <t>slices</t>
@@ -505,18 +502,12 @@
     <t>No</t>
   </si>
   <si>
-    <t>paving</t>
-  </si>
-  <si>
     <t>Meta tags permitted on all slices</t>
   </si>
   <si>
     <t>A string value indicating painted color for the slice (e.g. "red" is common for bus lanes, "green" or "blue" for bike lanes). Allow some other descriptive words for special patterns or artwork</t>
   </si>
   <si>
-    <t>curb_height</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -764,6 +755,36 @@
   </si>
   <si>
     <t xml:space="preserve">This denotes how start point transitions are defined in the specification. They are in the form: {index_position_of_connecting_street_slice: transition_type}. The index position indicates where the connecting slice is on the other street, and the transition type can have the values of : angled, s-shaped, offset, and semi-circle. </t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SharedStreets ID for the specific segment of a consolidated centerline (no dual carriageways). This should be a unique ID. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description: Represents a web readable geojson layer with both line geometry and nested slices identified. This helps create a web transferable layer for application development. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SharedStreets ID for the specific segment of a consolidated centerline (no dual carriageways). This should be a unique ID. When working with a crosswalk file, this ID can repeat. </t>
+  </si>
+  <si>
+    <t>RowIndex</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A numeric index starting at 0 to the number of slices in the current SharedStreetID segment. The RowIndex with a SharedStreetID should be a unique ID if used in combination. </t>
+  </si>
+  <si>
+    <t>This denotes any other metadata to be associated with the slice. Consists of a list of tags in the formate: "tag_name"=&gt;tag_value;"tag_name_2"=&gt;tag_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description: A share-row-crosswalk consists of each row representing a slice of a shared-street id. Intended to allow the conversion between Additive and Sliced based specifications in an editable GIS/SQL database. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description: Consists of a line geometry file that is a flat table consisting of standardized right of way description fields. Each shared-row-id considered unique, and represents a single consolidated centerline for a street (no dual carriageways). Provides a GIS/SQL compatible database schema. </t>
   </si>
 </sst>
 </file>
@@ -1146,7 +1167,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1162,6 +1183,11 @@
         <v>18</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>241</v>
+      </c>
+    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>0</v>
@@ -1196,7 +1222,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>117</v>
       </c>
@@ -1210,7 +1236,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>121</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1834,24 +1860,207 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F3E168-994C-406C-B158-8312D24CB96A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.62890625" customWidth="1"/>
+    <col min="2" max="2" width="50.3125" customWidth="1"/>
+    <col min="3" max="3" width="29.83984375" customWidth="1"/>
+    <col min="4" max="4" width="39.26171875" customWidth="1"/>
+    <col min="5" max="5" width="50.83984375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" t="s">
+        <v>237</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CE16D9-6B4A-4B97-84C9-4C29085A06C3}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1869,12 +2078,17 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>234</v>
+      </c>
+    </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>114</v>
@@ -1922,49 +2136,49 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>121</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -1976,13 +2190,13 @@
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -1994,42 +2208,60 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C12" s="2">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>131</v>
+        <v>232</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>136</v>
+      <c r="F14" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2042,8 +2274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14113956-9C41-4528-BBB9-AD2809B184AF}">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2057,23 +2289,23 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2087,334 +2319,334 @@
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>148</v>
+        <v>232</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F19" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D20" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F26" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D28" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D29" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D30" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D31" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2422,237 +2654,237 @@
     </row>
     <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F34" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
+        <v>192</v>
+      </c>
+      <c r="E37" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" t="s">
         <v>195</v>
-      </c>
-      <c r="E37" t="s">
-        <v>147</v>
-      </c>
-      <c r="F37" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F38" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F39" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
+        <v>196</v>
+      </c>
+      <c r="E40" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" t="s">
         <v>199</v>
-      </c>
-      <c r="E40" t="s">
-        <v>147</v>
-      </c>
-      <c r="F40" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F41" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F42" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F43" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F44" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F45" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="7" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F48" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F49" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F50" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F51" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F52" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F53" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F54" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E55" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
+        <v>211</v>
+      </c>
+      <c r="E56" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" t="s">
         <v>214</v>
-      </c>
-      <c r="E56" t="s">
-        <v>147</v>
-      </c>
-      <c r="F56" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="E57" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F57" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E58" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F58" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Add Meta Tags for Sidewalk Furniture & Through Zones
I think this is one way to support paths and other typeso of facilities.
This might require more review. Possibly, paths should be their own
characteristic rather than a trait of the sidewalk through zone. @louh -
Any thoughts on this?
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CB284F-5A18-4FC7-8979-30A3A9B0140B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DDF23F-0C9C-4EC1-A4FD-8C4DEA38A3D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="1332" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="258">
   <si>
     <t>Field name</t>
   </si>
@@ -248,9 +248,6 @@
     <t>Left_Sidewalk_Frontage_Zone</t>
   </si>
   <si>
-    <t>Width in meters of the Left sidewalk where pedestrians would walk.</t>
-  </si>
-  <si>
     <t>Left_Sidewalk_Through_Zone</t>
   </si>
   <si>
@@ -260,61 +257,34 @@
     <t>Left_Through_Lane_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Width in meters of the Left most drive lane closest to the curb. This can often be referred to as a curbside lane. If this type of lane does not exist, the value is zero. </t>
-  </si>
-  <si>
     <t>Left_Through_Lane_2</t>
   </si>
   <si>
-    <t xml:space="preserve">Width in meters of the second Left most drive lane. If this type of lane does not exist, the value is zero. </t>
-  </si>
-  <si>
     <t>Left_Through_Lane_3</t>
   </si>
   <si>
-    <t xml:space="preserve">Width in meters of the third Left most drive lane. If this type of lane does not exist, the value is zero. </t>
-  </si>
-  <si>
     <t>Left_Through_Lane_4</t>
   </si>
   <si>
-    <t xml:space="preserve">Width in meters of the fourth Left most drive lane. If this type of lane does not exist, the value is zero. </t>
-  </si>
-  <si>
     <t>Left_Through_Lane_X</t>
   </si>
   <si>
-    <t xml:space="preserve">Width in meters of any additional lanes that might be on the Left side of the street. The number will just increase to accommodate for an additive specification, but it is an optional element. If this type of lane does not exist, the value is zero. </t>
-  </si>
-  <si>
     <t>Left_Bike_Lane</t>
   </si>
   <si>
-    <t xml:space="preserve">Width of the Left bicycle lane in meters. </t>
-  </si>
-  <si>
     <t>Left_Bike_Buffer</t>
   </si>
   <si>
-    <t xml:space="preserve">Width in meters of a Left bicycle buffer. </t>
-  </si>
-  <si>
     <t>Left_Bike_Buffer_Meta</t>
   </si>
   <si>
     <t>Left_Parking_Lane</t>
   </si>
   <si>
-    <t xml:space="preserve">Width in meters of the Left parking lane. It is possible this zone is more complex than being just on-street parking, but it will be used to describe the width of a curbside zone that is not intended for traversal. </t>
-  </si>
-  <si>
     <t>Left_Parking_Lane_Meta</t>
   </si>
   <si>
     <t>Left_Transit_Lane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Width in meters of a Left transit lane dedicated to moving high occupancy modes such as bus lanes, HOV lanes, and other types of lane. Defaults to describing a bus lane. </t>
   </si>
   <si>
     <t>Left_Transit_Meta</t>
@@ -801,6 +771,75 @@
   </si>
   <si>
     <t>Double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of the right sidewalk between adjacent land uses and the pedestrian through zone. </t>
+  </si>
+  <si>
+    <t>Width in meters of the left sidewalk where pedestrians would walk.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of the left most drive lane closest to the curb. This can often be referred to as a curbside lane. If this type of lane does not exist, the value is zero. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of the second left most drive lane. If this type of lane does not exist, the value is zero. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of the third left most drive lane. If this type of lane does not exist, the value is zero. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of the fourth left most drive lane. If this type of lane does not exist, the value is zero. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of any additional lanes that might be on the left side of the street. The number will just increase to accommodate for an additive specification, but it is an optional element. If this type of lane does not exist, the value is zero. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width of the left bicycle lane in meters. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of a left bicycle buffer. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of the left parking lane. It is possible this zone is more complex than being just on-street parking, but it will be used to describe the width of a curbside zone that is not intended for traversal. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of a left transit lane dedicated to moving high occupancy modes such as bus lanes, HOV lanes, and other types of lane. Defaults to describing a bus lane. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of the left sidewalk between adjacent land uses and the pedestrian through zone. </t>
+  </si>
+  <si>
+    <t>Left_Sidewalk_Furniture_Meta</t>
+  </si>
+  <si>
+    <t>LSFW_Furn_M</t>
+  </si>
+  <si>
+    <t>This metatag descripts the type of furniture zone being placed based on the following categories: [street_trees_in_planted_buffer, street_trees_in_curb_cuts, planted_buffer, filter_buffer, transit_shelter, complex]</t>
+  </si>
+  <si>
+    <t>Right_Sidewalk_Furniture_Meta</t>
+  </si>
+  <si>
+    <t>RSFW_Furn_M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed based on the following categories: [street_trees_in_planted_buffer, street_trees_in_curb_cuts, planted_buffer, filter_buffer, transit_shelter, complex]. </t>
+  </si>
+  <si>
+    <t>Right_Sidewalk_Through_Meta</t>
+  </si>
+  <si>
+    <t>RSW_Thru_M</t>
+  </si>
+  <si>
+    <t>In cases where the lines being described are not typical concrete sidewalks, this can be used to described segments that have special properties such as paths or gravel segments. The following categories are possible: [concrete, ashpalt_path, gravel, compacted_soil]</t>
+  </si>
+  <si>
+    <t>Left_Sidewalk_Through_Meta</t>
+  </si>
+  <si>
+    <t>LSW_Thru_M</t>
   </si>
 </sst>
 </file>
@@ -1183,10 +1222,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1204,7 +1243,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1238,27 +1277,27 @@
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1272,7 +1311,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1292,29 +1331,29 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>253</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>254</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>6</v>
@@ -1323,32 +1362,32 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>250</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>251</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>29</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
@@ -1357,15 +1396,15 @@
         <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
@@ -1374,32 +1413,32 @@
         <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
@@ -1408,49 +1447,49 @@
         <v>2</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>6</v>
@@ -1459,15 +1498,15 @@
         <v>2</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>48</v>
@@ -1476,15 +1515,15 @@
         <v>15</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>6</v>
@@ -1493,15 +1532,15 @@
         <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>48</v>
@@ -1510,100 +1549,100 @@
         <v>15</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>6</v>
@@ -1612,32 +1651,32 @@
         <v>2</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>77</v>
+        <v>256</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>100</v>
+        <v>257</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>78</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>6</v>
@@ -1646,49 +1685,49 @@
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
-        <v>81</v>
+        <v>247</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>102</v>
+        <v>248</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>6</v>
@@ -1697,15 +1736,15 @@
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>6</v>
@@ -1714,66 +1753,66 @@
         <v>2</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>88</v>
+        <v>239</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>55</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B38" t="s">
-        <v>43</v>
+        <v>80</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>6</v>
@@ -1782,15 +1821,15 @@
         <v>2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B39" t="s">
-        <v>44</v>
+        <v>81</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>48</v>
@@ -1799,15 +1838,15 @@
         <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>6</v>
@@ -1816,58 +1855,126 @@
         <v>2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" t="s">
-        <v>61</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" t="s">
-        <v>48</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
-        <v>59</v>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>113</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1899,7 +2006,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -1933,66 +2040,66 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -2001,15 +2108,15 @@
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -2018,58 +2125,58 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2105,7 +2212,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2113,10 +2220,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2130,80 +2237,80 @@
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -2215,13 +2322,13 @@
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -2233,60 +2340,60 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C14" s="2">
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2302,7 +2409,7 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -2317,23 +2424,23 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2347,334 +2454,334 @@
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F14" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="9" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="F19" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="D20" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="F20" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="F22" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D23" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D24" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="D27" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D28" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="D29" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="D31" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2682,237 +2789,237 @@
     </row>
     <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="7" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="F34" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="7" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F37" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E38" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F38" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E39" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F39" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F40" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="E41" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F41" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="E42" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F42" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E43" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F43" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
+        <v>200</v>
+      </c>
+      <c r="E44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" t="s">
         <v>210</v>
-      </c>
-      <c r="E44" t="s">
-        <v>146</v>
-      </c>
-      <c r="F44" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E45" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F45" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="7" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="E48" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F48" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F49" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="E50" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F50" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F51" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E52" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F52" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F53" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="F54" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E55" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="E56" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F56" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E57" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F57" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="E58" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="F58" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2933,10 +3040,10 @@
   <sheetPr>
     <tabColor theme="0" tint="-4.9989318521683403E-2"/>
   </sheetPr>
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2948,10 +3055,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B1" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2962,13 +3069,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -2982,7 +3089,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -2996,105 +3103,105 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>253</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>244</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>250</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>244</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -3102,41 +3209,41 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="D13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
@@ -3144,10 +3251,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>48</v>
@@ -3158,13 +3265,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -3172,10 +3279,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>48</v>
@@ -3186,13 +3293,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>244</v>
+        <v>43</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
@@ -3200,41 +3307,41 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>244</v>
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>234</v>
       </c>
       <c r="D20" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>97</v>
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>244</v>
+        <v>48</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -3242,27 +3349,27 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -3270,27 +3377,27 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>77</v>
+        <v>256</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>244</v>
+        <v>48</v>
       </c>
       <c r="D24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -3298,13 +3405,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
-        <v>81</v>
+        <v>247</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>244</v>
+        <v>48</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -3312,27 +3419,27 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -3340,13 +3447,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D29" s="2">
         <v>0</v>
@@ -3354,55 +3461,55 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="D30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="D32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" t="s">
-        <v>43</v>
+        <v>80</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -3410,10 +3517,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B34" t="s">
-        <v>44</v>
+        <v>81</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>48</v>
@@ -3423,58 +3530,114 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
-        <v>56</v>
-      </c>
-      <c r="B35" t="s">
-        <v>60</v>
+      <c r="A35" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
         <v>57</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B40" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="D36" s="2">
+      <c r="C40" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D40" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
         <v>58</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B41" t="s">
         <v>62</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C41" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D41" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
         <v>59</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B42" t="s">
         <v>63</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C42" t="s">
         <v>48</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D42" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Replaced Sidewalk Through Meta with Off Street Tags
Replace sidewalk through metatags based on discussion with @louh  with
an Off_Street_Width and an Off_Street_Meta. Maybe this requires more
discussion in the future or edits, but for now we are not overloading
the sidewalk elements.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DDF23F-0C9C-4EC1-A4FD-8C4DEA38A3D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22614ECB-A5FF-451D-8DEE-9DCD97B365A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="259">
   <si>
     <t>Field name</t>
   </si>
@@ -827,19 +827,22 @@
     <t xml:space="preserve">This metatag descripts the type of furniture zone being placed based on the following categories: [street_trees_in_planted_buffer, street_trees_in_curb_cuts, planted_buffer, filter_buffer, transit_shelter, complex]. </t>
   </si>
   <si>
-    <t>Right_Sidewalk_Through_Meta</t>
-  </si>
-  <si>
-    <t>RSW_Thru_M</t>
-  </si>
-  <si>
-    <t>In cases where the lines being described are not typical concrete sidewalks, this can be used to described segments that have special properties such as paths or gravel segments. The following categories are possible: [concrete, ashpalt_path, gravel, compacted_soil]</t>
-  </si>
-  <si>
-    <t>Left_Sidewalk_Through_Meta</t>
-  </si>
-  <si>
-    <t>LSW_Thru_M</t>
+    <t>Off_Street_Width</t>
+  </si>
+  <si>
+    <t>Off_Street_Meta</t>
+  </si>
+  <si>
+    <t>Off_St_W</t>
+  </si>
+  <si>
+    <t>Off_St_M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of an off-street path facility or gravel road that does not have clear delinations for direction that runs parallel to the segment or is the segment being described (all other attributes are zero). </t>
+  </si>
+  <si>
+    <t>This describes the type of off-street facility being represented. Can be taken from the following categories: [asphalt, gravel, dirt]</t>
   </si>
 </sst>
 </file>
@@ -1222,10 +1225,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1331,22 +1334,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>255</v>
-      </c>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
@@ -1654,63 +1647,63 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>256</v>
+        <v>73</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>257</v>
+        <v>88</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
@@ -1719,15 +1712,15 @@
         <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>6</v>
@@ -1736,15 +1729,15 @@
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>6</v>
@@ -1753,49 +1746,49 @@
         <v>2</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>6</v>
@@ -1804,117 +1797,117 @@
         <v>2</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>55</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="E42" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B43" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>6</v>
@@ -1923,32 +1916,32 @@
         <v>2</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>6</v>
+        <v>62</v>
+      </c>
+      <c r="C45" t="s">
+        <v>48</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C46" t="s">
         <v>48</v>
@@ -1957,24 +1950,41 @@
         <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>253</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" t="s">
-        <v>48</v>
+        <v>255</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>103</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>254</v>
+      </c>
+      <c r="B48" t="s">
+        <v>256</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2409,8 +2419,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3042,8 +3052,8 @@
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3109,29 +3119,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>253</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>250</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>234</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -3139,13 +3149,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>250</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3153,10 +3163,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>234</v>
@@ -3167,10 +3177,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>234</v>
@@ -3181,10 +3191,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>234</v>
@@ -3195,38 +3205,38 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>234</v>
       </c>
       <c r="D11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>234</v>
       </c>
       <c r="D12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>234</v>
@@ -3237,97 +3247,97 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>234</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="D15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>234</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>54</v>
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="D17" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>234</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>234</v>
       </c>
       <c r="D19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>234</v>
+        <v>47</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
@@ -3335,38 +3345,38 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
+        <v>71</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>234</v>
       </c>
       <c r="D22" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>234</v>
@@ -3377,24 +3387,24 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>234</v>
@@ -3405,13 +3415,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
-        <v>247</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -3419,10 +3429,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>234</v>
@@ -3433,10 +3443,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>234</v>
@@ -3447,24 +3457,24 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>234</v>
       </c>
       <c r="D29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>234</v>
@@ -3475,38 +3485,38 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>234</v>
       </c>
       <c r="D31" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>234</v>
+        <v>48</v>
       </c>
       <c r="D32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>234</v>
@@ -3517,10 +3527,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>48</v>
@@ -3531,10 +3541,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>97</v>
+        <v>84</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>234</v>
@@ -3545,10 +3555,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>98</v>
+        <v>85</v>
+      </c>
+      <c r="B36" t="s">
+        <v>44</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>48</v>
@@ -3558,11 +3568,11 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="2" t="s">
-        <v>84</v>
+      <c r="A37" t="s">
+        <v>56</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>234</v>
@@ -3572,56 +3582,56 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="2" t="s">
-        <v>85</v>
+      <c r="A38" t="s">
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>48</v>
+        <v>234</v>
       </c>
       <c r="D38" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>234</v>
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>48</v>
       </c>
       <c r="D39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>234</v>
+        <v>63</v>
+      </c>
+      <c r="C40" t="s">
+        <v>48</v>
       </c>
       <c r="D40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>253</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
-      </c>
-      <c r="C41" t="s">
-        <v>48</v>
+        <v>255</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>234</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -3629,12 +3639,12 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>254</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
-      </c>
-      <c r="C42" t="s">
+        <v>256</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D42" s="2">

</xml_diff>

<commit_message>
Add Possible Value Column to Additive Spec
Possible values column added to Additive Spec. As we work on this, I am
starting to wonder if we should use coded values (Enums) instead of
text. If we add Domains to a database, it would be human readable
regardless. @louh  or @marsxul  any thoughts on this? I know GTFS does
this for some fields.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22614ECB-A5FF-451D-8DEE-9DCD97B365A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735A9900-B3C2-4DC5-BA72-ABAFB52B4A8C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="266">
   <si>
     <t>Field name</t>
   </si>
@@ -197,9 +197,6 @@
     <t>R_Prk_Meta</t>
   </si>
   <si>
-    <t>This describes the type of buffer that exists in the street based on the type. The possible categories are [paint,post,curb,planter].</t>
-  </si>
-  <si>
     <t>End_Crosswalk_Width</t>
   </si>
   <si>
@@ -224,12 +221,6 @@
     <t>B_X_W_Meta</t>
   </si>
   <si>
-    <t xml:space="preserve">This describes the parking parking zone type based on a few cateogories: [parking, passenger_loading,freight_loading,parklet]. It is not assumed that the entire curb is taken up by one of these uses, but just that it has atleast one of them. </t>
-  </si>
-  <si>
-    <t>This describes transit lane type from the following categories: [bus,hov,rail,]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Width in meters of the center lane or median that cannot be described by right or left. It typically refers to a median. </t>
   </si>
   <si>
@@ -242,9 +233,6 @@
     <t xml:space="preserve">Width in meters of the right parking lane. It is possible this zone is more complex than being just on-street parking, but it will be used to describe the width of a curbside zone that is not intended for traversal. </t>
   </si>
   <si>
-    <t>This describes the type of center lane from the following categories: [median,turn_lane,boulevard,barrier,median_turn_lane]</t>
-  </si>
-  <si>
     <t>Left_Sidewalk_Frontage_Zone</t>
   </si>
   <si>
@@ -336,12 +324,6 @@
   </si>
   <si>
     <t xml:space="preserve">SharedStreets geometry compliant LineString that is in WGS Coordinates. The orientation of right vs. left is based the the order of the vertices in this geometry, and its start and end points denote the crosswalk locations described in the specification. </t>
-  </si>
-  <si>
-    <t>This describes the type of crosswalk at the end of the segment from the following categories:[continental,transverse,ladder,textured,other]</t>
-  </si>
-  <si>
-    <t>This describes the type of crosswalk at the beginning of the segment from the following categories:[continental,transverse,ladder,textured,other]</t>
   </si>
   <si>
     <t>Level in JSON Hierarchy</t>
@@ -815,18 +797,12 @@
     <t>LSFW_Furn_M</t>
   </si>
   <si>
-    <t>This metatag descripts the type of furniture zone being placed based on the following categories: [street_trees_in_planted_buffer, street_trees_in_curb_cuts, planted_buffer, filter_buffer, transit_shelter, complex]</t>
-  </si>
-  <si>
     <t>Right_Sidewalk_Furniture_Meta</t>
   </si>
   <si>
     <t>RSFW_Furn_M</t>
   </si>
   <si>
-    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed based on the following categories: [street_trees_in_planted_buffer, street_trees_in_curb_cuts, planted_buffer, filter_buffer, transit_shelter, complex]. </t>
-  </si>
-  <si>
     <t>Off_Street_Width</t>
   </si>
   <si>
@@ -842,7 +818,52 @@
     <t xml:space="preserve">Width in meters of an off-street path facility or gravel road that does not have clear delinations for direction that runs parallel to the segment or is the segment being described (all other attributes are zero). </t>
   </si>
   <si>
-    <t>This describes the type of off-street facility being represented. Can be taken from the following categories: [asphalt, gravel, dirt]</t>
+    <t>Possible Values</t>
+  </si>
+  <si>
+    <t>This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised curb buffer), planter (temporary or permanent planter in buffer), separator (raised element placed intermittently along buffer).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This describes the parking parking zone type allowed. Categories include parking (personal vehicle storage), passenger_loading (passenger drop-off / loading) ,freight_loading (commercial vehicle drop-off / loading), parklet (mini-park or pedestrianized space) no-parking (no parking zone/fire lane/ etc.). It is not assumed that the entire curb is taken up by one of these uses, but just that it has atleast one of them. </t>
+  </si>
+  <si>
+    <t>parking;passenger_loading;freight_loading;parklet;no-parking</t>
+  </si>
+  <si>
+    <t>This describes transit lane type. The possible values include bus (bus only lane), hov (high occupancy vehicle lane), rail (light rail/street car lane), bus_bike (bus and bike shared lane).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This describes the type of right of way allocation typical to the center of a street. The options include a median (raised curb with no tapering for a turn lane), turn_lane (a two-way left turn lane), boulevard (a center lane allocation that tend to be large and contain pedestrian space of other lane allocations), barrier (a raised barrier such as a Jersey Barrier), median_turn_lane (a median with tapering at each intersection to accomodate left turn lanes). </t>
+  </si>
+  <si>
+    <t>This describes the type of off-street facility being represented. If the geometry represents an off-street path rather than a road or a road that has no formal delination, this tag along side Off_St_W can be used to represent a simplified rural road or path. The possible values are asphalt (impervious petroleum based path surface), gravel (loose aggregate material delinate path), dirt (compacted soil with little or no vegetation delinate path).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This describes the type of crosswalk at the end of the segment. The types of crosswalk that are possible are continental (high visibility bars spaced across intersection), transverse (standard two painted lines across intersection), ladder (combination of two painted lines and continental bars), textured (some type of custom colored &amp; textured pavement based crosswalk), other (other custom crosswalk design). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This describes the type of crosswalk at the beginning of the segment. The types of crosswalk that are possible are continental (high visibility bars spaced across intersection), transverse (standard two painted lines across intersection), ladder (combination of two painted lines and continental bars), textured (some type of custom colored &amp; textured pavement based crosswalk), other (other custom crosswalk design). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the cement), planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_buffer (placement of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
+  </si>
+  <si>
+    <t>paint;post;curb;planter;separator</t>
+  </si>
+  <si>
+    <t>median;turn_lane;boulevard;barrier;median_turn_lane</t>
+  </si>
+  <si>
+    <t>continental;transverse;ladder;textured;other</t>
+  </si>
+  <si>
+    <t>street_trees_in_planted_buffer;street_trees_in_curb_cuts;planted_buffer;filter_buffer;transit_shelter;complex</t>
+  </si>
+  <si>
+    <t>asphalt;gravel;dirt</t>
+  </si>
+  <si>
+    <t>bus;hov;rail;bus_bike</t>
   </si>
 </sst>
 </file>
@@ -917,7 +938,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -941,6 +962,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1225,10 +1249,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:C48"/>
+    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
+      <selection activeCell="F44" sqref="F6:F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1236,20 +1260,21 @@
     <col min="1" max="2" width="32.7890625" customWidth="1"/>
     <col min="3" max="3" width="20.89453125" customWidth="1"/>
     <col min="4" max="4" width="18.26171875" customWidth="1"/>
-    <col min="5" max="5" width="77.15625" customWidth="1"/>
+    <col min="5" max="5" width="51.15625" customWidth="1"/>
+    <col min="6" max="6" width="35.9453125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1265,8 +1290,11 @@
       <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="F5" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1280,27 +1308,33 @@
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>217</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1314,10 +1348,13 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>229</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1333,54 +1370,76 @@
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="F9" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>243</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>244</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>30</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>6</v>
@@ -1389,15 +1448,18 @@
         <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>29</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>6</v>
@@ -1406,15 +1468,18 @@
         <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>31</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
@@ -1423,49 +1488,58 @@
         <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>32</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>33</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>49</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>6</v>
@@ -1474,168 +1548,198 @@
         <v>2</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>65</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B24" t="s">
-        <v>44</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>2</v>
-      </c>
       <c r="E26" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>240</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>230</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>6</v>
@@ -1644,49 +1748,58 @@
         <v>2</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>17</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>73</v>
+        <v>241</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>88</v>
+        <v>242</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>231</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>6</v>
@@ -1695,15 +1808,18 @@
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>232</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>6</v>
@@ -1712,15 +1828,18 @@
         <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>233</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>6</v>
@@ -1729,49 +1848,58 @@
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>235</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>236</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>6</v>
@@ -1780,112 +1908,133 @@
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>237</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F42" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1899,27 +2048,33 @@
         <v>2</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>96</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>57</v>
       </c>
       <c r="B44" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>6</v>
+      <c r="C44" t="s">
+        <v>48</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>257</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -1933,59 +2088,87 @@
         <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>258</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>245</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
-      </c>
-      <c r="C46" t="s">
-        <v>48</v>
+        <v>247</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>249</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B47" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="s">
-        <v>254</v>
-      </c>
-      <c r="B48" t="s">
         <v>256</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>258</v>
-      </c>
+      <c r="F47" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F48" s="10"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F49" s="10"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F50" s="10"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F51" s="10"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F52" s="10"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F53" s="10"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F54" s="10"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F55" s="10"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F56" s="10"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F57" s="10"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F58" s="10"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F59" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2016,7 +2199,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2050,66 +2233,66 @@
         <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C6" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>6</v>
@@ -2118,15 +2301,15 @@
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -2135,58 +2318,58 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2222,7 +2405,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2230,10 +2413,10 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2247,80 +2430,80 @@
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -2332,13 +2515,13 @@
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -2350,60 +2533,60 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C14" s="2">
         <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2419,7 +2602,7 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="B5" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2434,23 +2617,23 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2464,334 +2647,334 @@
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E14" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F14" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D15" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D17" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="F19" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F20" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D25" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F26" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E27" t="s">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D28" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D29" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D30" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D31" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2799,237 +2982,237 @@
     </row>
     <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F34" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="7" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E37" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F37" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E38" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E39" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F39" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E40" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F40" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E41" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F41" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E42" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F42" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E43" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F43" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="E44" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F44" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="E45" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F45" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E48" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F48" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F49" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E50" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F50" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F51" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E52" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F52" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="F53" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="F54" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E55" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E56" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F56" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E57" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F57" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E58" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="F58" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3065,10 +3248,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B1" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3079,13 +3262,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -3099,7 +3282,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -3113,7 +3296,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -3127,7 +3310,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -3135,7 +3318,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -3155,7 +3338,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3169,7 +3352,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3183,7 +3366,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -3197,7 +3380,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -3211,7 +3394,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -3225,7 +3408,7 @@
         <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -3239,7 +3422,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -3267,7 +3450,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -3295,7 +3478,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -3323,7 +3506,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -3345,13 +3528,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -3359,13 +3542,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -3373,13 +3556,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -3387,10 +3570,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>48</v>
@@ -3401,13 +3584,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -3415,13 +3598,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -3429,13 +3612,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
@@ -3443,13 +3626,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -3457,13 +3640,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -3471,13 +3654,13 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
@@ -3485,13 +3668,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3499,10 +3682,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>48</v>
@@ -3513,13 +3696,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -3527,10 +3710,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>48</v>
@@ -3541,13 +3724,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
         <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -3555,7 +3738,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
         <v>44</v>
@@ -3569,13 +3752,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -3583,13 +3766,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -3597,10 +3780,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
         <v>48</v>
@@ -3611,10 +3794,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
         <v>48</v>
@@ -3625,13 +3808,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B41" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -3639,10 +3822,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B42" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Add Full Domain Script, Minor Edits
Minor edits and script changes to enable database to add domains to
geodatabases and feature classes.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735A9900-B3C2-4DC5-BA72-ABAFB52B4A8C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E362AC-C399-447F-BDE6-A3BAD4344AF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -957,14 +957,14 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1251,8 +1251,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
-      <selection activeCell="F44" sqref="F6:F47"/>
+    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1310,7 +1310,7 @@
       <c r="E6" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       <c r="E7" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1350,7 +1350,7 @@
       <c r="E8" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1370,7 +1370,7 @@
       <c r="E9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1390,7 +1390,7 @@
       <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       <c r="E11" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="8" t="s">
         <v>263</v>
       </c>
     </row>
@@ -1430,7 +1430,7 @@
       <c r="E12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1450,7 +1450,7 @@
       <c r="E13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
       <c r="E14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1490,7 +1490,7 @@
       <c r="E15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1510,7 +1510,7 @@
       <c r="E16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1530,7 +1530,7 @@
       <c r="E17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1550,7 +1550,7 @@
       <c r="E18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1570,7 +1570,7 @@
       <c r="E19" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>260</v>
       </c>
     </row>
@@ -1590,7 +1590,7 @@
       <c r="E20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1610,7 +1610,7 @@
       <c r="E21" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="8" t="s">
         <v>253</v>
       </c>
     </row>
@@ -1630,7 +1630,7 @@
       <c r="E22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1650,7 +1650,7 @@
       <c r="E23" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="8" t="s">
         <v>265</v>
       </c>
     </row>
@@ -1670,7 +1670,7 @@
       <c r="E24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1690,7 +1690,7 @@
       <c r="E25" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="8" t="s">
         <v>261</v>
       </c>
     </row>
@@ -1710,7 +1710,7 @@
       <c r="E26" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1730,7 +1730,7 @@
       <c r="E27" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
       <c r="E28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1770,7 +1770,7 @@
       <c r="E29" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="8" t="s">
         <v>263</v>
       </c>
     </row>
@@ -1790,7 +1790,7 @@
       <c r="E30" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1810,7 +1810,7 @@
       <c r="E31" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1830,7 +1830,7 @@
       <c r="E32" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1850,7 +1850,7 @@
       <c r="E33" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1870,7 +1870,7 @@
       <c r="E34" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1890,7 +1890,7 @@
       <c r="E35" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1910,7 +1910,7 @@
       <c r="E36" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1930,7 +1930,7 @@
       <c r="E37" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="8" t="s">
         <v>263</v>
       </c>
     </row>
@@ -1950,7 +1950,7 @@
       <c r="E38" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       <c r="E39" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="8" t="s">
         <v>253</v>
       </c>
     </row>
@@ -1990,7 +1990,7 @@
       <c r="E40" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2010,7 +2010,7 @@
       <c r="E41" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="F41" s="8" t="s">
         <v>265</v>
       </c>
     </row>
@@ -2030,7 +2030,7 @@
       <c r="E42" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2050,7 +2050,7 @@
       <c r="E43" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
       <c r="E44" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="8" t="s">
         <v>262</v>
       </c>
     </row>
@@ -2090,7 +2090,7 @@
       <c r="E45" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="F45" s="10" t="s">
+      <c r="F45" s="8" t="s">
         <v>262</v>
       </c>
     </row>
@@ -2110,7 +2110,7 @@
       <c r="E46" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2130,45 +2130,45 @@
       <c r="E47" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="8" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F48" s="10"/>
+      <c r="F48" s="8"/>
     </row>
     <row r="49" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F49" s="10"/>
+      <c r="F49" s="8"/>
     </row>
     <row r="50" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F50" s="10"/>
+      <c r="F50" s="8"/>
     </row>
     <row r="51" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F51" s="10"/>
+      <c r="F51" s="8"/>
     </row>
     <row r="52" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F52" s="10"/>
+      <c r="F52" s="8"/>
     </row>
     <row r="53" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F53" s="10"/>
+      <c r="F53" s="8"/>
     </row>
     <row r="54" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F54" s="10"/>
+      <c r="F54" s="8"/>
     </row>
     <row r="55" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F55" s="10"/>
+      <c r="F55" s="8"/>
     </row>
     <row r="56" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F56" s="10"/>
+      <c r="F56" s="8"/>
     </row>
     <row r="57" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F57" s="10"/>
+      <c r="F57" s="8"/>
     </row>
     <row r="58" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F58" s="10"/>
+      <c r="F58" s="8"/>
     </row>
     <row r="59" spans="6:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F59" s="10"/>
+      <c r="F59" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2754,10 +2754,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -2816,10 +2816,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B18" s="9"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Edits to Slice Spec
@louh  I changed the height parameter to be in CM instead of relative
heights. I just think this is more consistent with the spec, and we can
infer that from defaults divisors on the app side. Let me know if you
have any concerns.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E362AC-C399-447F-BDE6-A3BAD4344AF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0624A35-E336-47A3-81C5-F4B0C0458E24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
@@ -473,9 +473,6 @@
     <t>A string value indicating the paving material of the surface, e.g. "asphalt", "concrete", "cobblestone", "dirt", etc. (There should be some attempt at standardizing common values but allow custom values to be used.) This should not be a required value because specific slices can assume default values, e.g. the default value of paving for a drive_lane, if not specified, is "asphalt". Allow "none" if slice is not paved; e.g. plants, water</t>
   </si>
   <si>
-    <t>A relative number for the height of the surface. Rather than deal with specific measurements (which can vary depending on elevation and other factors) we (that is, Streetmix) uses 0 to indicate a road surface and 1 for a raised sidewalk surface. If there is no height difference between the drive_lane and sidewalk areas, the values will both be 0. A surface at half-curb-height is 0.5. Ditches are given negative values. Raised platforms can be given any number above 1 that represents a relative scale factor compared to the difference in height between the sidewalk curb and road surface (e.g. 2, 2.5, 3, etc)</t>
-  </si>
-  <si>
     <t>bike_lane</t>
   </si>
   <si>
@@ -864,6 +861,9 @@
   </si>
   <si>
     <t>bus;hov;rail;bus_bike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The height of the surface in centimeters relative to the road surface. While the geometry can encode Z coordinates for abolute elevation, this attribute specifically for knowning the vertical height of surfaces relative to the street. A typical curb can be 4 to 6 inches in height (10.2 - 15.2 cm), while just the asphalt road bed would be considered be at height 0. </t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1251,7 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B45" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1291,7 +1291,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1328,7 +1328,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>9</v>
@@ -1348,7 +1348,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>9</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="11" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
@@ -1408,10 +1408,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1568,10 +1568,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1608,10 +1608,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>252</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1648,10 +1648,10 @@
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1688,10 +1688,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1708,7 +1708,7 @@
         <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>9</v>
@@ -1728,7 +1728,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>9</v>
@@ -1756,10 +1756,10 @@
     </row>
     <row r="29" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>48</v>
@@ -1768,10 +1768,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1788,7 +1788,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>9</v>
@@ -1808,7 +1808,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>9</v>
@@ -1828,7 +1828,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>9</v>
@@ -1848,7 +1848,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>9</v>
@@ -1868,7 +1868,7 @@
         <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>9</v>
@@ -1888,7 +1888,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>9</v>
@@ -1908,7 +1908,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>9</v>
@@ -1928,10 +1928,10 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1948,7 +1948,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>9</v>
@@ -1968,10 +1968,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>252</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1988,7 +1988,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>9</v>
@@ -2008,10 +2008,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2068,10 +2068,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -2088,18 +2088,18 @@
         <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>6</v>
@@ -2108,7 +2108,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>9</v>
@@ -2116,10 +2116,10 @@
     </row>
     <row r="47" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B47" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -2128,10 +2128,10 @@
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2184,8 +2184,8 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2199,7 +2199,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2250,24 +2250,24 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C6" t="s">
         <v>220</v>
       </c>
-      <c r="B6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2340,10 +2340,10 @@
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>112</v>
@@ -2369,7 +2369,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2405,7 +2405,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2461,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2557,7 +2557,7 @@
     <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -2602,8 +2602,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2633,7 +2633,7 @@
         <v>122</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2660,7 +2660,7 @@
     <row r="7" spans="1:6" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
@@ -2689,7 +2689,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>110</v>
@@ -2702,13 +2702,13 @@
         <v>130</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>135</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
@@ -2718,14 +2718,14 @@
         <v>130</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>106</v>
@@ -2734,14 +2734,14 @@
         <v>130</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>106</v>
@@ -2750,19 +2750,19 @@
         <v>130</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2784,7 +2784,7 @@
         <v>124</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -2795,10 +2795,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2806,105 +2806,105 @@
         <v>124</v>
       </c>
       <c r="D17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" t="s">
+        <v>142</v>
+      </c>
+      <c r="F20" t="s">
         <v>165</v>
-      </c>
-      <c r="D20" t="s">
-        <v>143</v>
-      </c>
-      <c r="F20" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
+        <v>141</v>
+      </c>
+      <c r="D23" t="s">
         <v>142</v>
-      </c>
-      <c r="D23" t="s">
-        <v>143</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
       </c>
       <c r="F23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
       <c r="F24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
       <c r="F25" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2918,63 +2918,63 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
       <c r="F28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
       </c>
       <c r="F30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="F31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2982,139 +2982,139 @@
     </row>
     <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F34" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E37" t="s">
         <v>130</v>
       </c>
       <c r="F37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E38" t="s">
         <v>130</v>
       </c>
       <c r="F38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E39" t="s">
         <v>130</v>
       </c>
       <c r="F39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E40" t="s">
         <v>130</v>
       </c>
       <c r="F40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E41" t="s">
         <v>130</v>
       </c>
       <c r="F41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E42" t="s">
         <v>130</v>
       </c>
       <c r="F42" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E43" t="s">
         <v>130</v>
       </c>
       <c r="F43" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E44" t="s">
         <v>130</v>
       </c>
       <c r="F44" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E45" t="s">
         <v>130</v>
       </c>
       <c r="F45" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E48" t="s">
         <v>125</v>
       </c>
       <c r="F48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3122,18 +3122,18 @@
         <v>108</v>
       </c>
       <c r="F49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E50" t="s">
         <v>130</v>
       </c>
       <c r="F50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3141,18 +3141,18 @@
         <v>108</v>
       </c>
       <c r="F51" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E52" t="s">
         <v>130</v>
       </c>
       <c r="F52" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3160,59 +3160,59 @@
         <v>108</v>
       </c>
       <c r="F53" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" t="s">
+        <v>184</v>
+      </c>
+      <c r="F54" t="s">
         <v>185</v>
-      </c>
-      <c r="F54" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E55" t="s">
         <v>130</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E56" t="s">
         <v>130</v>
       </c>
       <c r="F56" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E57" t="s">
         <v>130</v>
       </c>
       <c r="F57" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E58" t="s">
         <v>130</v>
       </c>
       <c r="F58" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3248,10 +3248,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" t="s">
         <v>226</v>
-      </c>
-      <c r="B1" t="s">
-        <v>227</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3282,7 +3282,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -3296,7 +3296,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -3310,7 +3310,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -3338,7 +3338,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3352,7 +3352,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3366,7 +3366,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -3380,7 +3380,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -3394,7 +3394,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -3408,7 +3408,7 @@
         <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -3422,7 +3422,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -3450,7 +3450,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -3478,7 +3478,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -3506,7 +3506,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -3534,7 +3534,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -3548,7 +3548,7 @@
         <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -3562,7 +3562,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -3570,7 +3570,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>84</v>
@@ -3590,7 +3590,7 @@
         <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -3604,7 +3604,7 @@
         <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -3618,7 +3618,7 @@
         <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
@@ -3632,7 +3632,7 @@
         <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -3646,7 +3646,7 @@
         <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -3660,7 +3660,7 @@
         <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
@@ -3674,7 +3674,7 @@
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3702,7 +3702,7 @@
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -3730,7 +3730,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -3758,7 +3758,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -3772,7 +3772,7 @@
         <v>60</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -3808,13 +3808,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B41" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -3822,10 +3822,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B42" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Edits To Spec Sheet
Specify that right side of the street is for lanes towards end points,
and left is the reverse. Change filter_buffer to filter_strip. More is
needed to make the slice specification consistent with additive meta
tags.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9BDCC5-FD14-4FCD-8B31-CDDC0A667331}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48149FF-FDAC-4D17-980E-8CB19064A5E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="270">
   <si>
     <t>Field name</t>
   </si>
@@ -734,9 +734,6 @@
     <t xml:space="preserve">Description: A share-row-crosswalk consists of each row representing a slice of a shared-street id. Intended to allow the conversion between Additive and Sliced based specifications in an editable GIS/SQL database. </t>
   </si>
   <si>
-    <t xml:space="preserve">Description: Consists of a line geometry file that is a flat table consisting of standardized right of way description fields. Each shared-row-id considered unique, and represents a single consolidated centerline for a street (no dual carriageways). Provides a GIS/SQL compatible database schema. </t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -870,6 +867,15 @@
   </si>
   <si>
     <t>rowindex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the cement), planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placement of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
+  </si>
+  <si>
+    <t>street_trees_in_planted_buffer;street_trees_in_curb_cuts;planted_buffer;filter_strip;transit_shelter;complex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description: Consists of a line geometry file that is a flat table consisting of standardized right of way description fields. Each shared-row-id considered unique, and represents a single consolidated centerline for a street (no dual carriageways). Right oriented fields denote lanes enabling traffic in the forward direction towards the end point of the line, and left oriented fields denote lanes enabling traffic in the reverse direciton toward the start point of the line.  Provides a GIS/SQL compatible database schema. </t>
   </si>
 </sst>
 </file>
@@ -944,7 +950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -971,6 +977,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1257,8 +1266,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1275,10 +1284,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>222</v>
-      </c>
+    <row r="3" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
@@ -1297,7 +1311,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1354,7 +1368,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>9</v>
@@ -1402,10 +1416,10 @@
     </row>
     <row r="11" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>241</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
@@ -1414,10 +1428,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1574,10 +1588,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1614,10 +1628,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>249</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1654,10 +1668,10 @@
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1694,10 +1708,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1714,7 +1728,7 @@
         <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>9</v>
@@ -1734,7 +1748,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>9</v>
@@ -1762,10 +1776,10 @@
     </row>
     <row r="29" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>238</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>239</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>48</v>
@@ -1774,10 +1788,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1794,7 +1808,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>9</v>
@@ -1814,7 +1828,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>9</v>
@@ -1834,7 +1848,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>9</v>
@@ -1854,7 +1868,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>9</v>
@@ -1874,7 +1888,7 @@
         <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>9</v>
@@ -1894,7 +1908,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>9</v>
@@ -1914,7 +1928,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>9</v>
@@ -1934,10 +1948,10 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1954,7 +1968,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>9</v>
@@ -1974,10 +1988,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>249</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1994,7 +2008,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>9</v>
@@ -2014,10 +2028,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2074,10 +2088,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -2094,18 +2108,18 @@
         <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>6</v>
@@ -2114,7 +2128,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>9</v>
@@ -2122,10 +2136,10 @@
     </row>
     <row r="47" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -2134,10 +2148,10 @@
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2177,6 +2191,9 @@
       <c r="F59" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:F3"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2190,7 +2207,7 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -2261,7 +2278,7 @@
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B6" t="s">
         <v>217</v>
@@ -2324,7 +2341,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2390,7 +2407,7 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2539,7 +2556,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2608,7 +2625,7 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
@@ -2708,7 +2725,7 @@
         <v>129</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2724,7 +2741,7 @@
         <v>129</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -3254,10 +3271,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" t="s">
         <v>223</v>
-      </c>
-      <c r="B1" t="s">
-        <v>224</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3288,7 +3305,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -3302,7 +3319,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -3316,7 +3333,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -3324,7 +3341,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -3344,7 +3361,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3358,7 +3375,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3372,7 +3389,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -3386,7 +3403,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -3400,7 +3417,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -3414,7 +3431,7 @@
         <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -3428,7 +3445,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -3456,7 +3473,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -3484,7 +3501,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -3512,7 +3529,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -3540,7 +3557,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -3554,7 +3571,7 @@
         <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -3568,7 +3585,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -3576,7 +3593,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>84</v>
@@ -3596,7 +3613,7 @@
         <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -3610,7 +3627,7 @@
         <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -3624,7 +3641,7 @@
         <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
@@ -3638,7 +3655,7 @@
         <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -3652,7 +3669,7 @@
         <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -3666,7 +3683,7 @@
         <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
@@ -3680,7 +3697,7 @@
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3708,7 +3725,7 @@
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -3736,7 +3753,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -3764,7 +3781,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -3778,7 +3795,7 @@
         <v>60</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -3814,13 +3831,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B41" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -3828,10 +3845,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B42" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Adjust Specification to Match Slice More Closely
Adjust domain CSVs & specification sheet. Most change intended to match
the two specifications together.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA90EAB2-BFBB-4DC9-9BD4-9821632F720E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40DC3D7-097D-4368-97A5-1EE08B1BF7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="271">
   <si>
     <t>Field name</t>
   </si>
@@ -461,9 +461,6 @@
     <t>Meta tags permitted on all slices</t>
   </si>
   <si>
-    <t>A string value indicating painted color for the slice (e.g. "red" is common for bus lanes, "green" or "blue" for bike lanes). Allow some other descriptive words for special patterns or artwork</t>
-  </si>
-  <si>
     <t>Number</t>
   </si>
   <si>
@@ -551,9 +548,6 @@
     <t>Through-lane dedicated to bicycles or other vehicles of similar shape and speed.</t>
   </si>
   <si>
-    <t>Through-lane dedicated to pedestrians, usually (but not always) on a raised curb</t>
-  </si>
-  <si>
     <t>"Dedicated" means "primarily intended for." In each of these cases mixed traffic may be permitted and a meta tag will indicate what kind of mixing is allowed.</t>
   </si>
   <si>
@@ -569,9 +563,6 @@
     <t>A through-lane with fixed infrastructure (e.g. rail-based transit)</t>
   </si>
   <si>
-    <t>A string value indicating the type of rail transit (trolley, light rail, heavy rail)</t>
-  </si>
-  <si>
     <t>Whether the transit lane permits automobiles.</t>
   </si>
   <si>
@@ -581,9 +572,6 @@
     <t>bus_allowed</t>
   </si>
   <si>
-    <t>Whether the transit lane permits non-fixed-rail transit, e.g. buses</t>
-  </si>
-  <si>
     <t>see above</t>
   </si>
   <si>
@@ -608,30 +596,12 @@
     <t>passenger_loading</t>
   </si>
   <si>
-    <t>A loading zone, primarily for passenger pickup/dropoff.</t>
-  </si>
-  <si>
-    <t>A loading zone, primarily for the loading and unloading of goods</t>
-  </si>
-  <si>
-    <t>Any slice that has been reconfigured for a temporary purpose, e.g construction</t>
-  </si>
-  <si>
     <t>barrier_type</t>
   </si>
   <si>
-    <t>If the slice is a barrier, type of barrier (e.g. traffic cone, jersey barrier, fencing, etc)</t>
-  </si>
-  <si>
-    <t>What is this temporary purpose (e.g. construction, event)</t>
-  </si>
-  <si>
     <t>commercial</t>
   </si>
   <si>
-    <t>A zone where commerce is permitted, e.g. food trucks, farmer's markets, newstands</t>
-  </si>
-  <si>
     <t>transit_shelter</t>
   </si>
   <si>
@@ -656,18 +626,9 @@
     <t>A water channel</t>
   </si>
   <si>
-    <t>An area for plants, primarily for decorative purposes (though it can have an ecological impact). Usually placed in a sidewalk (as opposed to a median) This differentiates this from:</t>
-  </si>
-  <si>
     <t>filter_strip</t>
   </si>
   <si>
-    <t>An area designated for stormwater management, which is usually (but not required to be) vegetated.</t>
-  </si>
-  <si>
-    <t>Curb zones are the liminal space between through traffic and a pedestrian zone which have usually been reserved for automobile parking, but more recently, segments of the curb zone have been chopped up and designated for other uses. Therefore curb zones may be portions of slices from point A to B. Note that there is a very fine line between some types of uses in a curb zone and miscellaneous objects.</t>
-  </si>
-  <si>
     <t xml:space="preserve">A zone where some designated of bicycle parking will be placed. </t>
   </si>
   <si>
@@ -680,18 +641,12 @@
     <t xml:space="preserve">A zone where dockless bicycle shared or scooters can be parked. </t>
   </si>
   <si>
-    <t xml:space="preserve">The type of median allowed. Possible values include: cement, vegetated, vegetated with trees, stone, brick, other. </t>
-  </si>
-  <si>
     <t xml:space="preserve">A raised street slice whose elements  are in the center of the street. </t>
   </si>
   <si>
     <t xml:space="preserve">A raised street slice whose elements typically provide some degree of protection to a multimodal lane such as a bike lane. </t>
   </si>
   <si>
-    <t xml:space="preserve">The type of buffer allowed. Possible values include: cement, vegetated, vegetated with trees, stone, brick, other. </t>
-  </si>
-  <si>
     <t>Sub-Meta Tags</t>
   </si>
   <si>
@@ -701,12 +656,6 @@
     <t>start</t>
   </si>
   <si>
-    <t xml:space="preserve">This denotes how end point transitions are defined in the specification. They are in the form: {index_position_of_connecting_street_slice: transition_type}. The index position indicates where the connecting slice is on the other street, and the transition type can have the values of : angled, s-shaped, offset, and semi-circle. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This denotes how start point transitions are defined in the specification. They are in the form: {index_position_of_connecting_street_slice: transition_type}. The index position indicates where the connecting slice is on the other street, and the transition type can have the values of : angled, s-shaped, offset, and semi-circle. </t>
-  </si>
-  <si>
     <t>material</t>
   </si>
   <si>
@@ -824,33 +773,9 @@
     <t xml:space="preserve">This describes the type of right of way allocation typical to the center of a street. The options include a median (raised curb with no tapering for a turn lane), turn_lane (a two-way left turn lane), boulevard (a center lane allocation that tend to be large and contain pedestrian space of other lane allocations), barrier (a raised barrier such as a Jersey Barrier), median_turn_lane (a median with tapering at each intersection to accomodate left turn lanes). </t>
   </si>
   <si>
-    <t>This describes the type of off-street facility being represented. If the geometry represents an off-street path rather than a road or a road that has no formal delination, this tag along side Off_St_W can be used to represent a simplified rural road or path. The possible values are asphalt (impervious petroleum based path surface), gravel (loose aggregate material delinate path), dirt (compacted soil with little or no vegetation delinate path).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This describes the type of crosswalk at the end of the segment. The types of crosswalk that are possible are continental (high visibility bars spaced across intersection), transverse (standard two painted lines across intersection), ladder (combination of two painted lines and continental bars), textured (some type of custom colored &amp; textured pavement based crosswalk), other (other custom crosswalk design). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This describes the type of crosswalk at the beginning of the segment. The types of crosswalk that are possible are continental (high visibility bars spaced across intersection), transverse (standard two painted lines across intersection), ladder (combination of two painted lines and continental bars), textured (some type of custom colored &amp; textured pavement based crosswalk), other (other custom crosswalk design). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the cement), planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_buffer (placement of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
-  </si>
-  <si>
-    <t>paint;post;curb;planter;separator</t>
-  </si>
-  <si>
     <t>median;turn_lane;boulevard;barrier;median_turn_lane</t>
   </si>
   <si>
-    <t>continental;transverse;ladder;textured;other</t>
-  </si>
-  <si>
-    <t>street_trees_in_planted_buffer;street_trees_in_curb_cuts;planted_buffer;filter_buffer;transit_shelter;complex</t>
-  </si>
-  <si>
-    <t>asphalt;gravel;dirt</t>
-  </si>
-  <si>
     <t>bus;hov;rail;bus_bike</t>
   </si>
   <si>
@@ -860,25 +785,100 @@
     <t xml:space="preserve">Denotes the height in centimeters (cm) of the slice relative to the rest of the roadbed. </t>
   </si>
   <si>
-    <t xml:space="preserve">The height of the surface in centimeters relative to the road surface. While the geometry can encode Z coordinates for absolute elevation, this attribute specifically for knowing the vertical height of surfaces relative to the street. A typical curb can be 4 to 6 inches in height (10.2 - 15.2 cm), while just the asphalt road bed would be considered be at height 0. </t>
-  </si>
-  <si>
-    <t>Definition in flux, but these transition properties describe how the edge of one slice should transition to a neighboring slice based on some criteria. E.g. a drive_lane next to another_drive lane might have a transition of a broken white line. A raised curb next to an asphalt-paved slice might have a gutter, or a ramp, or other types of transitions.</t>
-  </si>
-  <si>
     <t>rowindex</t>
   </si>
   <si>
     <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the cement), planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placement of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
   </si>
   <si>
-    <t>street_trees_in_planted_buffer;street_trees_in_curb_cuts;planted_buffer;filter_strip;transit_shelter;complex</t>
-  </si>
-  <si>
     <t xml:space="preserve">Description: Consists of a line geometry file that is a flat table consisting of standardized right of way description fields. Each shared-row-id considered unique, and represents a single consolidated centerline for a street (no dual carriageways). Right oriented fields denote lanes enabling traffic in the forward direction towards the end point of the line, and left oriented fields denote lanes enabling traffic in the reverse direciton toward the start point of the line.  Provides a GIS/SQL compatible database schema. </t>
   </si>
   <si>
     <t xml:space="preserve">Denotes whether the slice is facing forward (towards the geometry end point) or reverse (towards the geometry start point). Possible values are forward, reverse, and bidirectional. </t>
+  </si>
+  <si>
+    <t>This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised cement curb buffer), planter (temporary or permanent planter in buffer), separator (raised element placed intermittently along buffer).</t>
+  </si>
+  <si>
+    <t>asphalt;gravel;dirt;stone;brick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This describes the type of off-street facility being represented. If the geometry represents an off-street path rather than a road or a road that has no formal delination, this tag along side Off_St_W can be used to represent a simplified rural road or path. The possible values are asphalt (impervious petroleum based path surface), gravel (loose aggregate material delinate path), dirt (compacted soil with little or no vegetation delinate path), stone (large cobblestone or other type of surface), brick (clay brick trail surface). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This describes the type of crosswalk at the beginning of the segment. The types of crosswalk that are possible are continental (high visibility bars spaced across intersection), transverse (standard two painted lines across intersection), ladder (combination of two painted lines and continental bars), textured (some type of custom colored &amp; textured pavement based crosswalk),zebra (combinatin of two painted lines and angled diagonal crossbars), other (other custom crosswalk design). </t>
+  </si>
+  <si>
+    <t>continental;transverse;ladder;textured;zebra;other</t>
+  </si>
+  <si>
+    <t>A string value indicating the paving material of the surface; e.g. "asphalt"; "concrete"; "cobblestone"; "dirt"; etc. (There should be some attempt at standardizing common values but allow custom values to be used.) This should not be a required value because specific slices can assume default values; e.g. the default value of paving for a drive_lane; if not specified; is "asphalt". Allow "none" if slice is not paved; e.g. plants; water</t>
+  </si>
+  <si>
+    <t>A string value indicating painted color for the slice (e.g. "red" is common for bus lanes; "green" or "blue" for bike lanes). Allow some other descriptive words for special patterns or artwork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The height of the surface in centimeters relative to the road surface. While the geometry can encode Z coordinates for absolute elevation; this attribute specifically for knowing the vertical height of surfaces relative to the street. A typical curb can be 4 to 6 inches in height (10.2 - 15.2 cm); while just the asphalt road bed would be considered be at height 0. </t>
+  </si>
+  <si>
+    <t>Definition in flux; but these transition properties describe how the edge of one slice should transition to a neighboring slice based on some criteria. E.g. a drive_lane next to another_drive lane might have a transition of a broken white line. A raised curb next to an asphalt-paved slice might have a gutter; or a ramp; or other types of transitions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This denotes how end point transitions are defined in the specification. They are in the form: {index_position_of_connecting_street_slice: transition_type}. The index position indicates where the connecting slice is on the other street; and the transition type can have the values of : angled; s-shaped; offset; and semi-circle. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This denotes how start point transitions are defined in the specification. They are in the form: {index_position_of_connecting_street_slice: transition_type}. The index position indicates where the connecting slice is on the other street; and the transition type can have the values of : angled; s-shaped; offset; and semi-circle. </t>
+  </si>
+  <si>
+    <t>Through-lane dedicated to pedestrians; usually (but not always) on a raised curb</t>
+  </si>
+  <si>
+    <t>A string value indicating the type of rail transit (trolley; light rail; heavy rail)</t>
+  </si>
+  <si>
+    <t>Whether the transit lane permits non-fixed-rail transit; e.g. buses</t>
+  </si>
+  <si>
+    <t>Curb zones are the liminal space between through traffic and a pedestrian zone which have usually been reserved for automobile parking; but more recently; segments of the curb zone have been chopped up and designated for other uses. Therefore curb zones may be portions of slices from point A to B. Note that there is a very fine line between some types of uses in a curb zone and miscellaneous objects.</t>
+  </si>
+  <si>
+    <t>A loading zone; primarily for the loading and unloading of goods</t>
+  </si>
+  <si>
+    <t>A loading zone; primarily for passenger pickup/dropoff.</t>
+  </si>
+  <si>
+    <t>A zone where commerce is permitted; e.g. food trucks; farmer's markets; newstands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of median allowed. Possible values include: paint;curb; vegetated; vegetated_with_trees; stone; brick; other. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of buffer allowed. Possible values include:  paint;post;curb;planter;separator;vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts; stone; brick; other. </t>
+  </si>
+  <si>
+    <t>Any slice that has been reconfigured for a temporary purpose; e.g construction</t>
+  </si>
+  <si>
+    <t>What is this temporary purpose (e.g. construction; event)</t>
+  </si>
+  <si>
+    <t>If the slice is a barrier; type of barrier (e.g. traffic cone; jersey barrier; fencing; etc)</t>
+  </si>
+  <si>
+    <t>An area for plants; primarily for decorative purposes (though it can have an ecological impact). Usually placed in a sidewalk (as opposed to a median).</t>
+  </si>
+  <si>
+    <t>The planting strip type describes the type of vegetated buffer provided. Possible values include:vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts</t>
+  </si>
+  <si>
+    <t>An area designated for stormwater management; which is usually (but not required to be) vegetated.</t>
+  </si>
+  <si>
+    <t>vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts;filter_strip;transit_shelter;complex</t>
+  </si>
+  <si>
+    <t>paint;post;curb;planter;separator;vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts; stone; brick; other</t>
   </si>
 </sst>
 </file>
@@ -975,14 +975,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1269,8 +1269,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1288,14 +1288,14 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
+      <c r="A3" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
@@ -1314,7 +1314,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1351,7 +1351,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>9</v>
@@ -1371,7 +1371,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>9</v>
@@ -1419,10 +1419,10 @@
     </row>
     <row r="11" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
@@ -1431,10 +1431,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>267</v>
+        <v>240</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1591,10 +1591,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>256</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1631,10 +1631,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1671,10 +1671,10 @@
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1711,10 +1711,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1731,7 +1731,7 @@
         <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>9</v>
@@ -1751,7 +1751,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>9</v>
@@ -1779,10 +1779,10 @@
     </row>
     <row r="29" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>238</v>
+        <v>221</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>48</v>
@@ -1791,10 +1791,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1811,7 +1811,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>9</v>
@@ -1831,7 +1831,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>228</v>
+        <v>211</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>9</v>
@@ -1851,7 +1851,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>9</v>
@@ -1871,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>9</v>
@@ -1891,7 +1891,7 @@
         <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>9</v>
@@ -1911,7 +1911,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>9</v>
@@ -1931,7 +1931,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>233</v>
+        <v>216</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>9</v>
@@ -1951,10 +1951,10 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1971,7 +1971,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>9</v>
@@ -1991,10 +1991,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2011,7 +2011,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>9</v>
@@ -2031,10 +2031,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2077,7 +2077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -2091,13 +2091,13 @@
         <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -2111,18 +2111,18 @@
         <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="B46" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>6</v>
@@ -2131,18 +2131,18 @@
         <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="B47" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -2151,10 +2151,10 @@
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2210,7 +2210,7 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2225,7 +2225,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2276,24 +2276,24 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
       <c r="B6" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2344,7 +2344,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2361,15 +2361,15 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>112</v>
@@ -2378,7 +2378,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2395,7 +2395,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -2431,7 +2431,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>215</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2487,7 +2487,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>214</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2559,7 +2559,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2583,7 +2583,7 @@
     <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -2595,7 +2595,7 @@
         <v>2</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2626,10 +2626,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2637,8 +2637,8 @@
     <col min="1" max="1" width="15.89453125" customWidth="1"/>
     <col min="2" max="3" width="20.3671875" customWidth="1"/>
     <col min="4" max="4" width="30.1015625" customWidth="1"/>
-    <col min="5" max="5" width="28.15625" customWidth="1"/>
-    <col min="6" max="6" width="76.1015625" customWidth="1"/>
+    <col min="5" max="5" width="10.5234375" customWidth="1"/>
+    <col min="6" max="6" width="91.734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2648,7 +2648,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2659,7 +2659,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2686,7 +2686,7 @@
     <row r="7" spans="1:6" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
@@ -2696,7 +2696,7 @@
         <v>129</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>133</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2712,7 +2712,7 @@
         <v>129</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>131</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2722,19 +2722,19 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>129</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>264</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
@@ -2744,14 +2744,14 @@
         <v>129</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>106</v>
@@ -2760,14 +2760,14 @@
         <v>129</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>106</v>
@@ -2776,19 +2776,19 @@
         <v>129</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>212</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="B13" s="9"/>
+      <c r="A13" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" s="10"/>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2801,7 +2801,7 @@
       <c r="E14" t="s">
         <v>124</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2810,21 +2810,21 @@
         <v>123</v>
       </c>
       <c r="D15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2832,105 +2832,106 @@
         <v>123</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="11" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="B18" s="10"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="5"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>135</v>
-      </c>
-      <c r="F19" t="s">
-        <v>161</v>
+        <v>134</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D20" t="s">
-        <v>141</v>
-      </c>
-      <c r="F20" t="s">
-        <v>164</v>
+        <v>140</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>139</v>
-      </c>
-      <c r="F22" t="s">
-        <v>159</v>
+        <v>138</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D23" t="s">
         <v>140</v>
-      </c>
-      <c r="D23" t="s">
-        <v>141</v>
       </c>
       <c r="E23" t="s">
         <v>15</v>
       </c>
-      <c r="F23" t="s">
-        <v>165</v>
+      <c r="F23" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E24" t="s">
         <v>15</v>
       </c>
-      <c r="F24" t="s">
-        <v>143</v>
+      <c r="F24" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E25" t="s">
         <v>15</v>
       </c>
-      <c r="F25" t="s">
-        <v>146</v>
+      <c r="F25" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>142</v>
-      </c>
-      <c r="F26" t="s">
-        <v>166</v>
+        <v>141</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2943,64 +2944,64 @@
       <c r="E27" t="s">
         <v>2</v>
       </c>
-      <c r="F27" t="s">
-        <v>167</v>
+      <c r="F27" s="2" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
-      <c r="F28" t="s">
-        <v>168</v>
+      <c r="F28" s="2" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D29" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
-      <c r="F29" t="s">
-        <v>171</v>
+      <c r="F29" s="2" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D30" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
       </c>
-      <c r="F30" t="s">
-        <v>172</v>
+      <c r="F30" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
-      <c r="F31" t="s">
-        <v>172</v>
+      <c r="F31" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3008,241 +3009,257 @@
     </row>
     <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>138</v>
-      </c>
-      <c r="F34" t="s">
-        <v>173</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>199</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E37" t="s">
         <v>129</v>
       </c>
-      <c r="F37" t="s">
-        <v>177</v>
+      <c r="F37" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="E38" t="s">
         <v>129</v>
       </c>
-      <c r="F38" t="s">
-        <v>175</v>
+      <c r="F38" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E39" t="s">
         <v>129</v>
       </c>
-      <c r="F39" t="s">
-        <v>176</v>
+      <c r="F39" s="2" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E40" t="s">
         <v>129</v>
       </c>
-      <c r="F40" t="s">
-        <v>181</v>
+      <c r="F40" s="2" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E41" t="s">
         <v>129</v>
       </c>
-      <c r="F41" t="s">
-        <v>180</v>
+      <c r="F41" s="2" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E42" t="s">
         <v>129</v>
       </c>
-      <c r="F42" t="s">
-        <v>187</v>
+      <c r="F42" s="2" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="E43" t="s">
         <v>129</v>
       </c>
-      <c r="F43" t="s">
-        <v>200</v>
+      <c r="F43" s="2" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="E44" t="s">
         <v>129</v>
       </c>
-      <c r="F44" t="s">
-        <v>202</v>
+      <c r="F44" s="2" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="E45" t="s">
         <v>129</v>
       </c>
-      <c r="F45" t="s">
-        <v>203</v>
-      </c>
+      <c r="F45" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F46" s="2"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="7" t="s">
-        <v>158</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="F47" s="2"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E48" t="s">
         <v>124</v>
       </c>
-      <c r="F48" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F48" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" t="s">
         <v>108</v>
       </c>
-      <c r="F49" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F49" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E50" t="s">
         <v>129</v>
       </c>
-      <c r="F50" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F50" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" t="s">
         <v>108</v>
       </c>
-      <c r="F51" t="s">
-        <v>207</v>
+      <c r="F51" s="2" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E52" t="s">
         <v>129</v>
       </c>
-      <c r="F52" t="s">
-        <v>182</v>
+      <c r="F52" s="2" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" t="s">
         <v>108</v>
       </c>
-      <c r="F53" t="s">
-        <v>185</v>
+      <c r="F53" s="2" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B54" t="s">
-        <v>183</v>
-      </c>
-      <c r="F54" t="s">
-        <v>184</v>
+        <v>176</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E55" t="s">
         <v>129</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="E56" t="s">
         <v>129</v>
       </c>
-      <c r="F56" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" t="s">
-        <v>197</v>
-      </c>
-      <c r="E57" t="s">
-        <v>129</v>
-      </c>
-      <c r="F57" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F56" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="E58" t="s">
         <v>129</v>
       </c>
-      <c r="F58" t="s">
-        <v>195</v>
+      <c r="F58" s="2" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="7"/>
+      <c r="A59" t="s">
+        <v>184</v>
+      </c>
+      <c r="E59" t="s">
+        <v>129</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="7"/>
+      <c r="F60" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3274,10 +3291,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3308,7 +3325,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -3322,7 +3339,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -3336,7 +3353,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -3344,7 +3361,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -3364,7 +3381,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3378,7 +3395,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3392,7 +3409,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -3406,7 +3423,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -3420,7 +3437,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -3434,7 +3451,7 @@
         <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -3448,7 +3465,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -3476,7 +3493,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -3504,7 +3521,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -3532,7 +3549,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -3560,7 +3577,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -3574,7 +3591,7 @@
         <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -3588,7 +3605,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -3596,7 +3613,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>84</v>
@@ -3616,7 +3633,7 @@
         <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -3630,7 +3647,7 @@
         <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -3644,7 +3661,7 @@
         <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
@@ -3658,7 +3675,7 @@
         <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -3672,7 +3689,7 @@
         <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -3686,7 +3703,7 @@
         <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
@@ -3700,7 +3717,7 @@
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3728,7 +3745,7 @@
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -3756,7 +3773,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -3784,7 +3801,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -3798,7 +3815,7 @@
         <v>60</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -3834,13 +3851,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
       <c r="B41" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -3848,10 +3865,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="B42" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Add Median With Turn Lane
This adds median with turn lane to the slice specification. This might
not work in all cases, but works in cases where the city starts with a
block to block representation of their streets. @louh  do you see this
as incompatible?
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40DC3D7-097D-4368-97A5-1EE08B1BF7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E65220-5B3C-482F-9635-B53A8A366F3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="274">
   <si>
     <t>Field name</t>
   </si>
@@ -788,18 +788,12 @@
     <t>rowindex</t>
   </si>
   <si>
-    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the cement), planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placement of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
-  </si>
-  <si>
     <t xml:space="preserve">Description: Consists of a line geometry file that is a flat table consisting of standardized right of way description fields. Each shared-row-id considered unique, and represents a single consolidated centerline for a street (no dual carriageways). Right oriented fields denote lanes enabling traffic in the forward direction towards the end point of the line, and left oriented fields denote lanes enabling traffic in the reverse direciton toward the start point of the line.  Provides a GIS/SQL compatible database schema. </t>
   </si>
   <si>
     <t xml:space="preserve">Denotes whether the slice is facing forward (towards the geometry end point) or reverse (towards the geometry start point). Possible values are forward, reverse, and bidirectional. </t>
   </si>
   <si>
-    <t>This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised cement curb buffer), planter (temporary or permanent planter in buffer), separator (raised element placed intermittently along buffer).</t>
-  </si>
-  <si>
     <t>asphalt;gravel;dirt;stone;brick</t>
   </si>
   <si>
@@ -879,6 +873,21 @@
   </si>
   <si>
     <t>paint;post;curb;planter;separator;vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts; stone; brick; other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the concrete), planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placoncrete of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
+  </si>
+  <si>
+    <t>This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised concrete curb buffer), planter (temporary or permanent planter in buffer), separator (raised element placed intermittently along buffer).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the concrete, planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placoncrete of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
+  </si>
+  <si>
+    <t>median_with_turn_lane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While this could be represented with a median and a turn-lane slice, this short hand indicates a center area that tapers with a turn lane at the end of it segments. The total width in this slice is how wide the median is at its widest point. </t>
   </si>
 </sst>
 </file>
@@ -1269,8 +1278,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1289,7 +1298,7 @@
     </row>
     <row r="3" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1431,10 +1440,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>240</v>
+        <v>269</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1591,10 +1600,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1791,10 +1800,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>240</v>
+        <v>271</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1954,7 +1963,7 @@
         <v>230</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2091,10 +2100,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -2111,10 +2120,10 @@
         <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2151,10 +2160,10 @@
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2361,7 +2370,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -2411,7 +2420,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2626,15 +2635,15 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.89453125" customWidth="1"/>
+    <col min="1" max="1" width="21.1015625" customWidth="1"/>
     <col min="2" max="3" width="20.3671875" customWidth="1"/>
     <col min="4" max="4" width="30.1015625" customWidth="1"/>
     <col min="5" max="5" width="10.5234375" customWidth="1"/>
@@ -2696,7 +2705,7 @@
         <v>129</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2712,7 +2721,7 @@
         <v>129</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2728,7 +2737,7 @@
         <v>129</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2744,7 +2753,7 @@
         <v>129</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2760,7 +2769,7 @@
         <v>129</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2776,7 +2785,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2854,7 +2863,7 @@
         <v>134</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2945,7 +2954,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2973,7 +2982,7 @@
         <v>15</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3024,12 +3033,12 @@
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="F35" s="2"/>
     </row>
-    <row r="36" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="7" t="s">
         <v>155</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3073,7 +3082,7 @@
         <v>129</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3084,7 +3093,7 @@
         <v>129</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3095,7 +3104,7 @@
         <v>129</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3156,18 +3165,15 @@
         <v>108</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>149</v>
-      </c>
-      <c r="E50" t="s">
-        <v>129</v>
+        <v>272</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>192</v>
+        <v>273</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3175,91 +3181,110 @@
         <v>108</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E52" t="s">
         <v>129</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" t="s">
         <v>108</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B54" t="s">
+      <c r="A54" t="s">
+        <v>150</v>
+      </c>
+      <c r="E54" t="s">
+        <v>129</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" t="s">
+        <v>108</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B56" t="s">
         <v>176</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" t="s">
+      <c r="F56" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
         <v>178</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E57" t="s">
         <v>129</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F57" s="4" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" t="s">
-        <v>183</v>
-      </c>
-      <c r="E56" t="s">
-        <v>129</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B57" t="s">
-        <v>108</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E58" t="s">
         <v>129</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59" t="s">
+        <v>108</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>186</v>
+      </c>
+      <c r="E60" t="s">
+        <v>129</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
         <v>184</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E61" t="s">
         <v>129</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F61" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="7"/>
-      <c r="F60" s="8"/>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="7"/>
+      <c r="F62" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add Path as Slice Type
Add shared use paths as a slice type.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E65220-5B3C-482F-9635-B53A8A366F3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400A9589-EF25-482F-BFCB-0B85B9C2C396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="278">
   <si>
     <t>Field name</t>
   </si>
@@ -572,9 +572,6 @@
     <t>bus_allowed</t>
   </si>
   <si>
-    <t>see above</t>
-  </si>
-  <si>
     <t>A specially designated through-lane intended for any non-automotive vehicle.</t>
   </si>
   <si>
@@ -827,9 +824,6 @@
     <t>Through-lane dedicated to pedestrians; usually (but not always) on a raised curb</t>
   </si>
   <si>
-    <t>A string value indicating the type of rail transit (trolley; light rail; heavy rail)</t>
-  </si>
-  <si>
     <t>Whether the transit lane permits non-fixed-rail transit; e.g. buses</t>
   </si>
   <si>
@@ -888,6 +882,24 @@
   </si>
   <si>
     <t xml:space="preserve">While this could be represented with a median and a turn-lane slice, this short hand indicates a center area that tapers with a turn lane at the end of it segments. The total width in this slice is how wide the median is at its widest point. </t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>A string value indicating the type of rail transit (trolley;light rail;heavy rail)</t>
+  </si>
+  <si>
+    <t>pedestrians_allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whether the path allows pedestrians. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A shared-use path intended for both bicycle and pedestrian traffic. </t>
+  </si>
+  <si>
+    <t>Whether the path allows bikes (may have a MUTCD bicycle stamp).</t>
   </si>
 </sst>
 </file>
@@ -1298,7 +1310,7 @@
     </row>
     <row r="3" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1323,7 +1335,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1360,7 +1372,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>9</v>
@@ -1380,7 +1392,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>9</v>
@@ -1428,10 +1440,10 @@
     </row>
     <row r="11" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
@@ -1440,10 +1452,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1600,10 +1612,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1640,10 +1652,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1680,10 +1692,10 @@
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1720,10 +1732,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1740,7 +1752,7 @@
         <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>9</v>
@@ -1760,7 +1772,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>9</v>
@@ -1788,10 +1800,10 @@
     </row>
     <row r="29" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>48</v>
@@ -1800,10 +1812,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1820,7 +1832,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>9</v>
@@ -1840,7 +1852,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>9</v>
@@ -1860,7 +1872,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>9</v>
@@ -1880,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>9</v>
@@ -1900,7 +1912,7 @@
         <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>9</v>
@@ -1920,7 +1932,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>9</v>
@@ -1940,7 +1952,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>9</v>
@@ -1960,10 +1972,10 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1980,7 +1992,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>9</v>
@@ -2000,10 +2012,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>231</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2020,7 +2032,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>9</v>
@@ -2040,10 +2052,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2100,10 +2112,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F44" s="8" t="s">
         <v>244</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -2120,18 +2132,18 @@
         <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>244</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>6</v>
@@ -2140,7 +2152,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>9</v>
@@ -2148,10 +2160,10 @@
     </row>
     <row r="47" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B47" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -2160,10 +2172,10 @@
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2234,7 +2246,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2285,24 +2297,24 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" t="s">
         <v>200</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2353,7 +2365,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2370,15 +2382,15 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>112</v>
@@ -2404,7 +2416,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2440,7 +2452,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2496,7 +2508,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2568,7 +2580,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2592,7 +2604,7 @@
     <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -2635,10 +2647,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2668,7 +2680,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2695,7 +2707,7 @@
     <row r="7" spans="1:6" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
@@ -2705,7 +2717,7 @@
         <v>129</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2721,7 +2733,7 @@
         <v>129</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2737,7 +2749,7 @@
         <v>129</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2753,14 +2765,14 @@
         <v>129</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>106</v>
@@ -2769,14 +2781,14 @@
         <v>129</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>106</v>
@@ -2785,7 +2797,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2863,7 +2875,7 @@
         <v>134</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2954,7 +2966,7 @@
         <v>2</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>253</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2982,7 +2994,7 @@
         <v>15</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2996,7 +3008,7 @@
         <v>15</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3010,62 +3022,73 @@
         <v>15</v>
       </c>
       <c r="F31" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>272</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" t="s">
+        <v>274</v>
+      </c>
+      <c r="D34" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F33" s="4"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>137</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F35" s="2"/>
-    </row>
-    <row r="36" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" s="7" t="s">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>170</v>
-      </c>
-      <c r="E37" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>180</v>
-      </c>
-      <c r="E38" t="s">
-        <v>129</v>
-      </c>
       <c r="F38" s="2" t="s">
-        <v>171</v>
+        <v>253</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="E39" t="s">
         <v>129</v>
@@ -3076,104 +3099,110 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E40" t="s">
         <v>129</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>256</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="E41" t="s">
         <v>129</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>257</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E42" t="s">
         <v>129</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E43" t="s">
         <v>129</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>187</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="E44" t="s">
         <v>129</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>189</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E45" t="s">
         <v>129</v>
       </c>
       <c r="F45" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>181</v>
+      </c>
+      <c r="E46" t="s">
+        <v>129</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>187</v>
+      </c>
+      <c r="E47" t="s">
+        <v>129</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>148</v>
+      </c>
+      <c r="E50" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>190</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="F47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" t="s">
-        <v>148</v>
-      </c>
-      <c r="E48" t="s">
-        <v>124</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49" t="s">
-        <v>108</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" t="s">
-        <v>272</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3181,18 +3210,15 @@
         <v>108</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>149</v>
-      </c>
-      <c r="E52" t="s">
-        <v>129</v>
+        <v>270</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>192</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3200,91 +3226,110 @@
         <v>108</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E54" t="s">
         <v>129</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" t="s">
         <v>108</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B56" t="s">
-        <v>176</v>
+      <c r="A56" t="s">
+        <v>150</v>
+      </c>
+      <c r="E56" t="s">
+        <v>129</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B58" t="s">
+        <v>175</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>177</v>
+      </c>
+      <c r="E59" t="s">
+        <v>129</v>
+      </c>
+      <c r="F59" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E57" t="s">
-        <v>129</v>
-      </c>
-      <c r="F57" s="4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" t="s">
-        <v>183</v>
-      </c>
-      <c r="E58" t="s">
-        <v>129</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B59" t="s">
-        <v>108</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E60" t="s">
         <v>129</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B61" t="s">
+        <v>108</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>185</v>
+      </c>
+      <c r="E62" t="s">
+        <v>129</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>183</v>
+      </c>
+      <c r="E63" t="s">
+        <v>129</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E61" t="s">
-        <v>129</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="7"/>
-      <c r="F62" s="8"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="7"/>
+      <c r="F64" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3316,10 +3361,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B1" t="s">
         <v>205</v>
-      </c>
-      <c r="B1" t="s">
-        <v>206</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3350,7 +3395,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -3364,7 +3409,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -3378,7 +3423,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -3386,7 +3431,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -3406,7 +3451,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3420,7 +3465,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3434,7 +3479,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -3448,7 +3493,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -3462,7 +3507,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -3476,7 +3521,7 @@
         <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -3490,7 +3535,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -3518,7 +3563,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -3546,7 +3591,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -3574,7 +3619,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -3602,7 +3647,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -3616,7 +3661,7 @@
         <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -3630,7 +3675,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -3638,7 +3683,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>84</v>
@@ -3658,7 +3703,7 @@
         <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -3672,7 +3717,7 @@
         <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -3686,7 +3731,7 @@
         <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
@@ -3700,7 +3745,7 @@
         <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -3714,7 +3759,7 @@
         <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -3728,7 +3773,7 @@
         <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
@@ -3742,7 +3787,7 @@
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3770,7 +3815,7 @@
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -3798,7 +3843,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -3826,7 +3871,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -3840,7 +3885,7 @@
         <v>60</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -3876,13 +3921,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -3890,10 +3935,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Add Turn Lane Modifications
@louh   per our discussion I added conditionally required tags that get
added to the turn lane slice if there is a block to block
representation. This still enables what I am looking for, but provides a
format consistent with the specification. Let me know what you think of
these edits.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400A9589-EF25-482F-BFCB-0B85B9C2C396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103CA333-D6D0-4813-8B26-FAFD1E48BC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,6 +15,7 @@
     <sheet name="Additive_Fields_Arc" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="287">
   <si>
     <t>Field name</t>
   </si>
@@ -521,9 +522,6 @@
     <t>temporary</t>
   </si>
   <si>
-    <t>A lane where automobiles are taken out of traffic flow in order to queue for turning</t>
-  </si>
-  <si>
     <t>A turn_lane may have a sharrow stamp</t>
   </si>
   <si>
@@ -878,12 +876,6 @@
     <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the concrete, planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placoncrete of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
   </si>
   <si>
-    <t>median_with_turn_lane</t>
-  </si>
-  <si>
-    <t xml:space="preserve">While this could be represented with a median and a turn-lane slice, this short hand indicates a center area that tapers with a turn lane at the end of it segments. The total width in this slice is how wide the median is at its widest point. </t>
-  </si>
-  <si>
     <t>path</t>
   </si>
   <si>
@@ -900,6 +892,42 @@
   </si>
   <si>
     <t>Whether the path allows bikes (may have a MUTCD bicycle stamp).</t>
+  </si>
+  <si>
+    <t>end_depth</t>
+  </si>
+  <si>
+    <t>begin_depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A lane where automobiles are taken out of traffic flow in order to queue for turning. These lanes are considered to be center-running and can be bidirectional if they represent a block to block segment with end and begin depths for symmetrical intersection end points (no additional turn lanes on either end of the segment). Segments should be split if one block has varying turn lanes counts. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This specifies the turn lane depth for the end point of the existing segment. If blank, it is assumed the turn lane is the depth of the entire length of the represented segment. For block to block representations, this parameter is required, and only works for symetrical end points of intersections. </t>
+  </si>
+  <si>
+    <t>Conditionally Required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This specifies the turn lane depth for the start point of the existing segment. If blank, it is assumed the turn lane is the depth of the entire length of the represented segment. For block to block representations, this parameter is required, and only works for symetrical end points of intersections. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This specifies the movements allowed at the turn. They are represented by a "|" delimited list of strings with the possible values of: left,right,through. </t>
+  </si>
+  <si>
+    <t>end_movements_allowed</t>
+  </si>
+  <si>
+    <t>begin_movements_allowed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This specifies the direction of the non-turnlane element after a transition ends. If none, assumed to be bidirectional. </t>
+  </si>
+  <si>
+    <t>remainder_allocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This specifies the allocation that remains in between turn lane pockets. If blank, it is assumed to be a median.  Otherwise, it can take on the properties of a slice type outlined in the specification. For block to block segments, this parameter is required unless the turn lanes takes up the full length of the segment. </t>
   </si>
 </sst>
 </file>
@@ -1310,7 +1338,7 @@
     </row>
     <row r="3" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1335,7 +1363,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1372,7 +1400,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>9</v>
@@ -1392,7 +1420,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>9</v>
@@ -1440,10 +1468,10 @@
     </row>
     <row r="11" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
@@ -1452,10 +1480,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1612,10 +1640,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1652,10 +1680,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1692,10 +1720,10 @@
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1732,10 +1760,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1752,7 +1780,7 @@
         <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>9</v>
@@ -1772,7 +1800,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>9</v>
@@ -1800,10 +1828,10 @@
     </row>
     <row r="29" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>48</v>
@@ -1812,10 +1840,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1832,7 +1860,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>9</v>
@@ -1852,7 +1880,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>9</v>
@@ -1872,7 +1900,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>9</v>
@@ -1892,7 +1920,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>9</v>
@@ -1912,7 +1940,7 @@
         <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>9</v>
@@ -1932,7 +1960,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>9</v>
@@ -1952,7 +1980,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>9</v>
@@ -1972,10 +2000,10 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1992,7 +2020,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>9</v>
@@ -2012,10 +2040,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2032,7 +2060,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>9</v>
@@ -2052,10 +2080,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2112,10 +2140,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F44" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -2132,18 +2160,18 @@
         <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>243</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B46" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>6</v>
@@ -2152,7 +2180,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>9</v>
@@ -2160,10 +2188,10 @@
     </row>
     <row r="47" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B47" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -2172,10 +2200,10 @@
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2232,7 +2260,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2246,7 +2274,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2266,7 +2294,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2297,24 +2325,24 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B6" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" t="s">
         <v>199</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2365,7 +2393,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2382,15 +2410,15 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>112</v>
@@ -2416,7 +2444,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2452,7 +2480,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2508,7 +2536,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2580,7 +2608,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2604,7 +2632,7 @@
     <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -2647,10 +2675,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2658,7 +2686,7 @@
     <col min="1" max="1" width="21.1015625" customWidth="1"/>
     <col min="2" max="3" width="20.3671875" customWidth="1"/>
     <col min="4" max="4" width="30.1015625" customWidth="1"/>
-    <col min="5" max="5" width="10.5234375" customWidth="1"/>
+    <col min="5" max="5" width="13.41796875" style="2" customWidth="1"/>
     <col min="6" max="6" width="91.734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2680,7 +2708,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2704,10 +2732,10 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
@@ -2717,7 +2745,7 @@
         <v>129</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2733,7 +2761,7 @@
         <v>129</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2749,7 +2777,7 @@
         <v>129</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2765,14 +2793,14 @@
         <v>129</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>106</v>
@@ -2781,14 +2809,14 @@
         <v>129</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>106</v>
@@ -2797,19 +2825,19 @@
         <v>129</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2819,7 +2847,7 @@
       <c r="D14" t="s">
         <v>112</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>124</v>
       </c>
       <c r="F14" s="2" t="s">
@@ -2833,19 +2861,19 @@
       <c r="D15" t="s">
         <v>140</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>136</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>151</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2855,146 +2883,152 @@
       <c r="D17" t="s">
         <v>140</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" t="s">
+        <v>275</v>
+      </c>
+      <c r="D18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" t="s">
+        <v>276</v>
+      </c>
+      <c r="D19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" t="s">
+        <v>282</v>
+      </c>
+      <c r="D20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" t="s">
+        <v>283</v>
+      </c>
+      <c r="D21" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" t="s">
+        <v>285</v>
+      </c>
+      <c r="D22" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="11" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="5"/>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="5"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
         <v>134</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" t="s">
+      <c r="F25" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" t="s">
+        <v>140</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D20" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+    </row>
+    <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
         <v>133</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
+      <c r="F27" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
         <v>138</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" t="s">
-        <v>139</v>
-      </c>
-      <c r="D23" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" t="s">
-        <v>143</v>
-      </c>
-      <c r="D24" t="s">
-        <v>140</v>
-      </c>
-      <c r="E24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B25" t="s">
-        <v>144</v>
-      </c>
-      <c r="D25" t="s">
-        <v>140</v>
-      </c>
-      <c r="E25" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" t="s">
-        <v>112</v>
-      </c>
-      <c r="E27" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" t="s">
-        <v>166</v>
-      </c>
-      <c r="D28" t="s">
-        <v>140</v>
-      </c>
-      <c r="E28" t="s">
-        <v>15</v>
-      </c>
       <c r="F28" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="D29" t="s">
         <v>140</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>252</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3004,7 +3038,7 @@
       <c r="D30" t="s">
         <v>140</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F30" s="2" t="s">
@@ -3018,7 +3052,7 @@
       <c r="D31" t="s">
         <v>140</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F31" s="2" t="s">
@@ -3027,314 +3061,376 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>272</v>
+        <v>141</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>276</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="D33" t="s">
-        <v>140</v>
-      </c>
-      <c r="E33" t="s">
-        <v>15</v>
+        <v>112</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" t="s">
-        <v>274</v>
+        <v>165</v>
       </c>
       <c r="D34" t="s">
         <v>140</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F35" s="4"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
-        <v>137</v>
+      <c r="B36" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" t="s">
+        <v>140</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="7" t="s">
+      <c r="B37" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" t="s">
+        <v>140</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>269</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" t="s">
+        <v>271</v>
+      </c>
+      <c r="D40" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>169</v>
-      </c>
-      <c r="E39" t="s">
-        <v>129</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" t="s">
-        <v>179</v>
-      </c>
-      <c r="E40" t="s">
-        <v>129</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" t="s">
-        <v>146</v>
-      </c>
-      <c r="E41" t="s">
-        <v>129</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>171</v>
-      </c>
+      <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>173</v>
-      </c>
-      <c r="E42" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>254</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" t="s">
-        <v>174</v>
-      </c>
-      <c r="E43" t="s">
-        <v>129</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
-        <v>176</v>
-      </c>
-      <c r="E44" t="s">
-        <v>129</v>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>180</v>
-      </c>
-      <c r="E45" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>181</v>
-      </c>
-      <c r="E46" t="s">
+        <v>178</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>187</v>
-      </c>
-      <c r="E47" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>129</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F48" s="2"/>
+      <c r="A48" t="s">
+        <v>172</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="F49" s="2"/>
+      <c r="A49" t="s">
+        <v>173</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>148</v>
-      </c>
-      <c r="E50" t="s">
-        <v>124</v>
+        <v>175</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" t="s">
-        <v>108</v>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>179</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>270</v>
+        <v>180</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53" t="s">
-        <v>108</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>186</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A54" t="s">
-        <v>149</v>
-      </c>
-      <c r="E54" t="s">
-        <v>129</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B55" t="s">
-        <v>108</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>258</v>
-      </c>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>150</v>
-      </c>
-      <c r="E56" t="s">
-        <v>129</v>
+        <v>148</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" t="s">
         <v>108</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B58" t="s">
-        <v>175</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>149</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" t="s">
-        <v>177</v>
-      </c>
-      <c r="E59" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B59" t="s">
+        <v>108</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>150</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="F59" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" t="s">
-        <v>182</v>
-      </c>
-      <c r="E60" t="s">
-        <v>129</v>
-      </c>
       <c r="F60" s="2" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" t="s">
         <v>108</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" t="s">
-        <v>185</v>
-      </c>
-      <c r="E62" t="s">
-        <v>129</v>
+      <c r="B62" t="s">
+        <v>174</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
+        <v>176</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" t="s">
+        <v>181</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B65" t="s">
+        <v>108</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" t="s">
+        <v>184</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" t="s">
+        <v>182</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E63" t="s">
-        <v>129</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="7"/>
-      <c r="F64" s="8"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="7"/>
+      <c r="F68" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3361,10 +3457,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" t="s">
         <v>204</v>
-      </c>
-      <c r="B1" t="s">
-        <v>205</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3387,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -3395,13 +3491,13 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -3409,13 +3505,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -3423,7 +3519,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -3431,7 +3527,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -3451,7 +3547,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3465,7 +3561,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3479,7 +3575,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -3493,7 +3589,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -3507,7 +3603,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -3521,7 +3617,7 @@
         <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -3535,7 +3631,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -3563,7 +3659,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -3591,7 +3687,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -3619,7 +3715,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -3647,7 +3743,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -3661,7 +3757,7 @@
         <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -3675,7 +3771,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -3683,7 +3779,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>84</v>
@@ -3703,7 +3799,7 @@
         <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -3717,7 +3813,7 @@
         <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -3731,7 +3827,7 @@
         <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
@@ -3745,7 +3841,7 @@
         <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -3759,7 +3855,7 @@
         <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -3773,7 +3869,7 @@
         <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
@@ -3787,7 +3883,7 @@
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3815,7 +3911,7 @@
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -3843,7 +3939,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -3871,7 +3967,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -3885,7 +3981,7 @@
         <v>60</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -3921,13 +4017,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -3935,10 +4031,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Add Bollard Type, Describe Buffers
Add Better descriptions, and add a bollard type of buffer. Bollards for
rigid structures providing physical separation in buffers.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103CA333-D6D0-4813-8B26-FAFD1E48BC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A44033-5B3F-4970-B0DB-D583814DB084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,6 @@
     <sheet name="Additive_Fields_Arc" sheetId="5" state="hidden" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="286">
   <si>
     <t>Field name</t>
   </si>
@@ -753,9 +752,6 @@
     <t>Possible Values</t>
   </si>
   <si>
-    <t>This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised curb buffer), planter (temporary or permanent planter in buffer), separator (raised element placed intermittently along buffer).</t>
-  </si>
-  <si>
     <t xml:space="preserve">This describes the parking parking zone type allowed. Categories include parking (personal vehicle storage), passenger_loading (passenger drop-off / loading) ,freight_loading (commercial vehicle drop-off / loading), parklet (mini-park or pedestrianized space) no-parking (no parking zone/fire lane/ etc.). It is not assumed that the entire curb is taken up by one of these uses, but just that it has atleast one of them. </t>
   </si>
   <si>
@@ -840,9 +836,6 @@
     <t xml:space="preserve">The type of median allowed. Possible values include: paint;curb; vegetated; vegetated_with_trees; stone; brick; other. </t>
   </si>
   <si>
-    <t xml:space="preserve">The type of buffer allowed. Possible values include:  paint;post;curb;planter;separator;vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts; stone; brick; other. </t>
-  </si>
-  <si>
     <t>Any slice that has been reconfigured for a temporary purpose; e.g construction</t>
   </si>
   <si>
@@ -864,15 +857,9 @@
     <t>vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts;filter_strip;transit_shelter;complex</t>
   </si>
   <si>
-    <t>paint;post;curb;planter;separator;vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts; stone; brick; other</t>
-  </si>
-  <si>
     <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the concrete), planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placoncrete of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
   </si>
   <si>
-    <t>This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised concrete curb buffer), planter (temporary or permanent planter in buffer), separator (raised element placed intermittently along buffer).</t>
-  </si>
-  <si>
     <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the concrete, planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placoncrete of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
   </si>
   <si>
@@ -928,6 +915,15 @@
   </si>
   <si>
     <t xml:space="preserve">This specifies the allocation that remains in between turn lane pockets. If blank, it is assumed to be a median.  Otherwise, it can take on the properties of a slice type outlined in the specification. For block to block segments, this parameter is required unless the turn lanes takes up the full length of the segment. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The type of buffer allowed. Possible values include:  paint;post;curb;planter;separator;vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts; stone;bollard;brick; other. </t>
+  </si>
+  <si>
+    <t>paint;post;curb;planter;separator;vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts; stone;brick;bollard;other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised concrete curb buffer), planter (temporary or permanent planter in buffer),vegetated(curb buffer with vegetation or grass),vegetated_with_trees (curb buffer with trees or other vegetation in the buffer),vegetated_with_tree_curb_cuts(curb buffers with vegetation and trees with gaps),stone (large stones delinating the buffer),brick (raised brick inset in a curb buffer),bollard (rigid post separating bicyclists from traffic), separator (raised element placed intermittently along buffer), and other (some other buffer type). </t>
   </si>
 </sst>
 </file>
@@ -1318,8 +1314,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1338,7 +1334,7 @@
     </row>
     <row r="3" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1480,10 +1476,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1626,7 +1622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1640,10 +1636,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>267</v>
+        <v>285</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1680,10 +1676,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1720,10 +1716,10 @@
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1760,10 +1756,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>232</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1840,10 +1836,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1986,7 +1982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:6" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
         <v>77</v>
       </c>
@@ -2000,10 +1996,10 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>228</v>
+        <v>285</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>265</v>
+        <v>284</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2040,10 +2036,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2080,10 +2076,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2140,10 +2136,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F44" s="8" t="s">
         <v>242</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -2160,10 +2156,10 @@
         <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>242</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2200,10 +2196,10 @@
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2330,7 +2326,7 @@
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B6" t="s">
         <v>198</v>
@@ -2393,7 +2389,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2410,7 +2406,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -2459,7 +2455,7 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2608,7 +2604,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2677,8 +2673,8 @@
   </sheetPr>
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="B49" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2745,7 +2741,7 @@
         <v>129</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2761,7 +2757,7 @@
         <v>129</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2777,7 +2773,7 @@
         <v>129</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2793,7 +2789,7 @@
         <v>129</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2809,7 +2805,7 @@
         <v>129</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2825,7 +2821,7 @@
         <v>129</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2873,7 +2869,7 @@
         <v>136</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2892,72 +2888,72 @@
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D19" t="s">
         <v>131</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D20" t="s">
         <v>112</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D21" t="s">
         <v>112</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D22" t="s">
         <v>112</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2971,7 +2967,7 @@
         <v>15</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2987,7 +2983,7 @@
         <v>134</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3078,7 +3074,7 @@
         <v>2</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3106,7 +3102,7 @@
         <v>15</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3139,10 +3135,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
+        <v>265</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3156,12 +3152,12 @@
         <v>15</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D40" t="s">
         <v>140</v>
@@ -3170,7 +3166,7 @@
         <v>15</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3195,7 +3191,7 @@
         <v>154</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3239,7 +3235,7 @@
         <v>129</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3250,7 +3246,7 @@
         <v>129</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3261,7 +3257,7 @@
         <v>129</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3322,7 +3318,7 @@
         <v>108</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3341,7 +3337,7 @@
         <v>108</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>257</v>
+        <v>283</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3352,7 +3348,7 @@
         <v>129</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3360,7 +3356,7 @@
         <v>108</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3368,7 +3364,7 @@
         <v>174</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3390,7 +3386,7 @@
         <v>129</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3398,7 +3394,7 @@
         <v>108</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3409,7 +3405,7 @@
         <v>129</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Minor Edit to Buffer Description
Minor Edit to description.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A44033-5B3F-4970-B0DB-D583814DB084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8E7E42-249E-4EBB-A376-AD66463D66F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -923,7 +923,7 @@
     <t>paint;post;curb;planter;separator;vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts; stone;brick;bollard;other</t>
   </si>
   <si>
-    <t xml:space="preserve">This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised concrete curb buffer), planter (temporary or permanent planter in buffer),vegetated(curb buffer with vegetation or grass),vegetated_with_trees (curb buffer with trees or other vegetation in the buffer),vegetated_with_tree_curb_cuts(curb buffers with vegetation and trees with gaps),stone (large stones delinating the buffer),brick (raised brick inset in a curb buffer),bollard (rigid post separating bicyclists from traffic), separator (raised element placed intermittently along buffer), and other (some other buffer type). </t>
+    <t xml:space="preserve">This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised concrete curb buffer), planter (temporary or permanent planter in buffer),vegetated(curb buffer with vegetation or grass),vegetated_with_trees (curb buffer with trees or other vegetation in the buffer),vegetated_with_tree_curb_cuts(curb buffers with vegetation and trees with gaps),stone (large stones delinating the buffer),brick (raised brick inset in a curb buffer),bollard (rigid post separating bicyclists from traffic), separator (raised element placed intermittently along buffer such as parking stops or zebra domes), and other (some other buffer type). </t>
   </si>
 </sst>
 </file>
@@ -1314,8 +1314,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1622,7 +1622,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:6" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:6" ht="187.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="2" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Minor Edit to Possible Values
Nothing added, just minor file edit.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8E7E42-249E-4EBB-A376-AD66463D66F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95FB7E3-E00F-42FB-A4B9-9C90491E501C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -854,9 +854,6 @@
     <t>An area designated for stormwater management; which is usually (but not required to be) vegetated.</t>
   </si>
   <si>
-    <t>vegetated; vegetated_with_trees;vegetated_with_tree_curb_cuts;filter_strip;transit_shelter;complex</t>
-  </si>
-  <si>
     <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the concrete), planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placoncrete of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
   </si>
   <si>
@@ -924,6 +921,9 @@
   </si>
   <si>
     <t xml:space="preserve">This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised concrete curb buffer), planter (temporary or permanent planter in buffer),vegetated(curb buffer with vegetation or grass),vegetated_with_trees (curb buffer with trees or other vegetation in the buffer),vegetated_with_tree_curb_cuts(curb buffers with vegetation and trees with gaps),stone (large stones delinating the buffer),brick (raised brick inset in a curb buffer),bollard (rigid post separating bicyclists from traffic), separator (raised element placed intermittently along buffer such as parking stops or zebra domes), and other (some other buffer type). </t>
+  </si>
+  <si>
+    <t>vegetated;vegetated_with_trees;vegetated_with_tree_curb_cuts;filter_strip;transit_shelter;complex</t>
   </si>
 </sst>
 </file>
@@ -1314,8 +1314,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1476,10 +1476,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1636,10 +1636,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1836,10 +1836,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1996,10 +1996,10 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2869,7 +2869,7 @@
         <v>136</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2888,72 +2888,72 @@
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D19" t="s">
         <v>131</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>275</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D20" t="s">
         <v>112</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D21" t="s">
         <v>112</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D22" t="s">
         <v>112</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2967,7 +2967,7 @@
         <v>15</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3074,7 +3074,7 @@
         <v>2</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3135,10 +3135,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3152,12 +3152,12 @@
         <v>15</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D40" t="s">
         <v>140</v>
@@ -3166,7 +3166,7 @@
         <v>15</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3337,7 +3337,7 @@
         <v>108</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Rearrange folder, Minor Edits
Rearrange ArcGIS Folders, Delete Old Files, Add Test Geojson, Minor edit
to excel sheet to specify that spec fields appear in properties.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C94B466-6884-4D47-BF88-B01593EF2D73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0358E083-682A-4F18-94FC-B4AAF987C9F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="288">
   <si>
     <t>Field name</t>
   </si>
@@ -369,9 +369,6 @@
   </si>
   <si>
     <t>String</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denotes from left to right, slices of a right of way, whose subattributes denote  its characteristics.The main sub-attribute are the type of slices (drive_lane, bike_lane,walkway, etc), its width in meters, its height in meters, its direction (forward or reverse), and a meta-data tag with other information about the slice (color, improvement year, or other information). </t>
   </si>
   <si>
     <t>meta</t>
@@ -924,6 +921,15 @@
   </si>
   <si>
     <t>This denotes any other metadata to be associated with the slice. Consists of a list of tags in the format: {"tag_name":tag_value;"tag_name_2":tag_value}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denotes from left to right, slices of a right of way, whose subattributes denote  its characteristics.The main sub-attribute are the type of slices (drive_lane, bike_lane,walkway, etc), its width in meters, its height in meters, its direction (forward or reverse), and a meta-data tag with other information about the slice (color, improvement year, or other information). These JSON slices will be located in the properties of the GEOJSON. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SharedStreets ID for the specific segment of a consolidated centerline (no dual carriageways). This should be a unique ID. This field will be located in the properties of the GEOJSON. </t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1314,8 +1320,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1334,7 +1340,7 @@
     </row>
     <row r="3" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1359,7 +1365,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1396,7 +1402,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>9</v>
@@ -1416,7 +1422,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>9</v>
@@ -1464,10 +1470,10 @@
     </row>
     <row r="11" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>220</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
@@ -1476,10 +1482,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1636,10 +1642,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1676,10 +1682,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>227</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1716,10 +1722,10 @@
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1756,10 +1762,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1776,7 +1782,7 @@
         <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>9</v>
@@ -1796,7 +1802,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>9</v>
@@ -1824,10 +1830,10 @@
     </row>
     <row r="29" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>218</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>48</v>
@@ -1836,10 +1842,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1856,7 +1862,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>9</v>
@@ -1876,7 +1882,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>9</v>
@@ -1896,7 +1902,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>9</v>
@@ -1916,7 +1922,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>9</v>
@@ -1936,7 +1942,7 @@
         <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>9</v>
@@ -1956,7 +1962,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>9</v>
@@ -1976,7 +1982,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>9</v>
@@ -1996,10 +2002,10 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2016,7 +2022,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>9</v>
@@ -2036,10 +2042,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>227</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2056,7 +2062,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>9</v>
@@ -2076,10 +2082,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2136,10 +2142,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F44" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -2156,18 +2162,18 @@
         <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>6</v>
@@ -2176,7 +2182,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>9</v>
@@ -2184,10 +2190,10 @@
     </row>
     <row r="47" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -2196,10 +2202,10 @@
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2255,8 +2261,8 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2270,7 +2276,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2321,24 +2327,24 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C6" t="s">
         <v>198</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="D6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2355,7 +2361,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2372,7 +2378,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2389,7 +2395,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2406,15 +2412,15 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>112</v>
@@ -2423,15 +2429,15 @@
         <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>112</v>
@@ -2440,7 +2446,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -2455,8 +2461,8 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2476,7 +2482,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2517,7 +2523,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="2" t="s">
         <v>104</v>
       </c>
@@ -2532,10 +2538,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="2" t="s">
         <v>105</v>
       </c>
@@ -2550,10 +2556,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>108</v>
@@ -2568,7 +2574,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>117</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2586,7 +2592,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2604,7 +2610,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2622,13 +2628,13 @@
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -2640,12 +2646,12 @@
         <v>2</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C14" s="2">
         <v>2</v>
@@ -2657,7 +2663,7 @@
         <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2688,23 +2694,23 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2718,46 +2724,46 @@
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
         <v>112</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
         <v>112</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2767,193 +2773,193 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>106</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" t="s">
         <v>112</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>273</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D20" t="s">
         <v>112</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D21" t="s">
         <v>112</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D22" t="s">
         <v>112</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2967,12 +2973,12 @@
         <v>15</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="5"/>
@@ -2980,87 +2986,87 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>160</v>
-      </c>
-      <c r="D26" t="s">
-        <v>140</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
+        <v>138</v>
+      </c>
+      <c r="D29" t="s">
         <v>139</v>
-      </c>
-      <c r="D29" t="s">
-        <v>140</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3074,113 +3080,113 @@
         <v>2</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D34" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3188,109 +3194,109 @@
     </row>
     <row r="44" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3298,19 +3304,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3318,18 +3324,18 @@
         <v>108</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3337,18 +3343,18 @@
         <v>108</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3356,37 +3362,37 @@
         <v>108</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
+        <v>175</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F63" s="4" t="s">
         <v>176</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -3394,29 +3400,29 @@
         <v>108</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
+        <v>181</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3453,10 +3459,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" t="s">
         <v>202</v>
-      </c>
-      <c r="B1" t="s">
-        <v>203</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3487,7 +3493,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -3501,7 +3507,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -3515,7 +3521,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -3523,7 +3529,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -3543,7 +3549,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3557,7 +3563,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3571,7 +3577,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -3585,7 +3591,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -3599,7 +3605,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -3613,7 +3619,7 @@
         <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -3627,7 +3633,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -3655,7 +3661,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -3683,7 +3689,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -3711,7 +3717,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -3739,7 +3745,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -3753,7 +3759,7 @@
         <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -3767,7 +3773,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -3775,7 +3781,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>84</v>
@@ -3795,7 +3801,7 @@
         <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -3809,7 +3815,7 @@
         <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -3823,7 +3829,7 @@
         <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
@@ -3837,7 +3843,7 @@
         <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -3851,7 +3857,7 @@
         <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -3865,7 +3871,7 @@
         <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
@@ -3879,7 +3885,7 @@
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3907,7 +3913,7 @@
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -3935,7 +3941,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -3963,7 +3969,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -3977,7 +3983,7 @@
         <v>60</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -4013,13 +4019,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -4027,10 +4033,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Change Parking Meta, Minor Edits
Change parking meta to match closer to CurbLR (SharedStreets suggested
values). Ensure match between additive & slice. Modify domain tools
accordingly. Minor spelling and grammar edits.
</commit_message>
<xml_diff>
--- a/specification/Shared-Row.xlsx
+++ b/specification/Shared-Row.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A99BD1-BF64-4877-885C-578DF0623FAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E03A74-9307-47FC-AC30-3D4AF314D9B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Additive Cross-section Spec" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="295">
   <si>
     <t>Field name</t>
   </si>
@@ -581,27 +581,18 @@
     <t>Generic designation for a curb zone with varying uses.</t>
   </si>
   <si>
-    <t>freight_loading</t>
-  </si>
-  <si>
     <t>passenger_loading</t>
   </si>
   <si>
     <t>barrier_type</t>
   </si>
   <si>
-    <t>commercial</t>
-  </si>
-  <si>
     <t>transit_shelter</t>
   </si>
   <si>
     <t>An area / platform for waiting for transit</t>
   </si>
   <si>
-    <t>auto_parking</t>
-  </si>
-  <si>
     <t>bike_parking</t>
   </si>
   <si>
@@ -740,18 +731,9 @@
     <t>Off_St_M</t>
   </si>
   <si>
-    <t xml:space="preserve">Width in meters of an off-street path facility or gravel road that does not have clear delinations for direction that runs parallel to the segment or is the segment being described (all other attributes are zero). </t>
-  </si>
-  <si>
     <t>Possible Values</t>
   </si>
   <si>
-    <t xml:space="preserve">This describes the parking parking zone type allowed. Categories include parking (personal vehicle storage), passenger_loading (passenger drop-off / loading) ,freight_loading (commercial vehicle drop-off / loading), parklet (mini-park or pedestrianized space) no-parking (no parking zone/fire lane/ etc.). It is not assumed that the entire curb is taken up by one of these uses, but just that it has atleast one of them. </t>
-  </si>
-  <si>
-    <t>parking;passenger_loading;freight_loading;parklet;no-parking</t>
-  </si>
-  <si>
     <t>This describes transit lane type. The possible values include bus (bus only lane), hov (high occupancy vehicle lane), rail (light rail/street car lane), bus_bike (bus and bike shared lane).</t>
   </si>
   <si>
@@ -779,12 +761,6 @@
     <t>asphalt;gravel;dirt;stone;brick</t>
   </si>
   <si>
-    <t xml:space="preserve">This describes the type of off-street facility being represented. If the geometry represents an off-street path rather than a road or a road that has no formal delination, this tag along side Off_St_W can be used to represent a simplified rural road or path. The possible values are asphalt (impervious petroleum based path surface), gravel (loose aggregate material delinate path), dirt (compacted soil with little or no vegetation delinate path), stone (large cobblestone or other type of surface), brick (clay brick trail surface). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This describes the type of crosswalk at the beginning of the segment. The types of crosswalk that are possible are continental (high visibility bars spaced across intersection), transverse (standard two painted lines across intersection), ladder (combination of two painted lines and continental bars), textured (some type of custom colored &amp; textured pavement based crosswalk),zebra (combinatin of two painted lines and angled diagonal crossbars), other (other custom crosswalk design). </t>
-  </si>
-  <si>
     <t>continental;transverse;ladder;textured;zebra;other</t>
   </si>
   <si>
@@ -818,18 +794,9 @@
     <t>A loading zone; primarily for the loading and unloading of goods</t>
   </si>
   <si>
-    <t>A loading zone; primarily for passenger pickup/dropoff.</t>
-  </si>
-  <si>
-    <t>A zone where commerce is permitted; e.g. food trucks; farmer's markets; newstands</t>
-  </si>
-  <si>
     <t xml:space="preserve">The type of median allowed. Possible values include: paint;curb; vegetated; vegetated_with_trees; stone; brick; other. </t>
   </si>
   <si>
-    <t>Any slice that has been reconfigured for a temporary purpose; e.g construction</t>
-  </si>
-  <si>
     <t>What is this temporary purpose (e.g. construction; event)</t>
   </si>
   <si>
@@ -845,12 +812,6 @@
     <t>An area designated for stormwater management; which is usually (but not required to be) vegetated.</t>
   </si>
   <si>
-    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the concrete), planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placoncrete of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the concrete, planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placoncrete of bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
-  </si>
-  <si>
     <t>path</t>
   </si>
   <si>
@@ -878,15 +839,9 @@
     <t xml:space="preserve">A lane where automobiles are taken out of traffic flow in order to queue for turning. These lanes are considered to be center-running and can be bidirectional if they represent a block to block segment with end and begin depths for symmetrical intersection end points (no additional turn lanes on either end of the segment). Segments should be split if one block has varying turn lanes counts. </t>
   </si>
   <si>
-    <t xml:space="preserve">This specifies the turn lane depth for the end point of the existing segment. If blank, it is assumed the turn lane is the depth of the entire length of the represented segment. For block to block representations, this parameter is required, and only works for symetrical end points of intersections. </t>
-  </si>
-  <si>
     <t>Conditionally Required</t>
   </si>
   <si>
-    <t xml:space="preserve">This specifies the turn lane depth for the start point of the existing segment. If blank, it is assumed the turn lane is the depth of the entire length of the represented segment. For block to block representations, this parameter is required, and only works for symetrical end points of intersections. </t>
-  </si>
-  <si>
     <t xml:space="preserve">This specifies the movements allowed at the turn. They are represented by a "|" delimited list of strings with the possible values of: left,right,through. </t>
   </si>
   <si>
@@ -927,6 +882,75 @@
   </si>
   <si>
     <t xml:space="preserve">Denotes the height in centimeters (cm) of the slice relative to the rest of the road. Defaults to 0. </t>
+  </si>
+  <si>
+    <t>commercial_loading</t>
+  </si>
+  <si>
+    <t>construction_zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A zone that indicates there is currently construction taking up space. </t>
+  </si>
+  <si>
+    <t>tow_away_zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A zone where tow-away rules are in place at nearly all times. </t>
+  </si>
+  <si>
+    <t>parking</t>
+  </si>
+  <si>
+    <t>commercial_activity</t>
+  </si>
+  <si>
+    <t>transit_stop</t>
+  </si>
+  <si>
+    <t>A location that is reserved for public transit vehicle loading, unloading, and dwelling.</t>
+  </si>
+  <si>
+    <t>parking;passenger_loading;commericial_loading;parklet;bike_share;dockless_parking;bike_parking;tow_away_zone;commercial_activity;transit_stop;construction_zone;flex_zone</t>
+  </si>
+  <si>
+    <t>This describes the parking parking zone type allowed. Categories include parking (personal vehicle storage), passenger_loading (passenger drop-off / loading) ,commercial_loading (commercial vehicle drop-off / loading), parklet (mini-park or pedestrianized space, bike_share (bike share stations or stalls), dockless_parking (spots to allocate dockless scooter/bike parking),bike_parking (locations for bike parking stands), tow_away_zone (no parking zone/fire lane/ etc.),transit_stop (location for transit stop loading/unloading/dwelling), construction_zone (a zone temporarily allocated to construction activity), flex_zone(a parking zone that can be different things at different times). It is not assumed that the entire curb is taken up by one of these uses, but just that it has at least one of them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This metatag descripts the type of furniture zone being placed. The possible values include street_trees_in_planted_buffer (denotes spaced trees placed in a long vegetated buffer), street_trees_in_curb_cuts (denotes spaced trees in cuts in the concrete), planted_buffer (denotes a grass or other semi-vegetated buffer along furniture zone), filter_strip (placement of  a bioswale or dipped catchment area for rain water in furniture zone), transit_shelter (denotes that a transit shelter is in the furniture zone), complex (denotes multiple types of objects in furniture zone perhaps better described by smaller segments in the slice specification). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SharedStreets geometry compliant LineString that is in WGS Coordinates. The orientation of right vs. left is based the  order of the vertices in this geometry, and its start and end points denote the crosswalk locations described in the specification. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This describes the type of buffer that exists in the street based on the type. Categories include paint (paint only buffers), post (flexible posts in a painted buffer), curb (raised concrete curb buffer), planter (temporary or permanent planter in buffer),vegetated(curb buffer with vegetation or grass),vegetated_with_trees (curb buffer with trees or other vegetation in the buffer),vegetated_with_tree_curb_cuts(curb buffers with vegetation and trees with gaps),stone (large stones delineating the buffer),brick (raised brick inset in a curb buffer),bollard (rigid post separating bicyclists from traffic), separator (raised element placed intermittently along buffer such as parking stops or zebra domes), and other (some other buffer type). </t>
+  </si>
+  <si>
+    <t>This describes the parking parking zone type allowed. Categories include parking (personal vehicle storage), passenger_loading (passenger drop-off / loading) ,commercial_loading (commercial vehicle drop-off / loading), parklet (mini-park or pedestrianized space, bike_share (bike share stations or stalls), dockless_parking (spots to allocate dockless scooter/bike parking),bike_parking (locations for bike parking stands), tow_away_zone (no parking zone/fire lane/ etc.),transit_stop (location for transit stop loading/unloading/dwelling), construction_zone(a zone temporarily allocated to construction activity), flex_zone(a parking zone that can be different things at different times). It is not assumed that the entire curb is taken up by one of these uses, but just that it has at least one of them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This describes the type of crosswalk at the beginning of the segment. The types of crosswalk that are possible are continental (high visibility bars spaced across intersection), transverse (standard two painted lines across intersection), ladder (combination of two painted lines and continental bars), textured (some type of custom colored &amp; textured pavement based crosswalk),zebra (combination of two painted lines and angled diagonal crossbars), other (other custom crosswalk design). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Width in meters of an off-street path facility or gravel road that does not have clear delineations for direction that runs parallel to the segment or is the segment being described (all other attributes are zero). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This describes the type of off-street facility being represented. If the geometry represents an off-street path rather than a road or a road that has no formal delineation, this tag along side Off_St_W can be used to represent a simplified rural road or path. The possible values are asphalt (impervious petroleum based path surface), gravel (loose aggregate material delineate path), dirt (compacted soil with little or no vegetation delineate path), stone (large cobblestone or other type of surface), brick (clay brick trail surface). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This specifies the turn lane depth for the end point of the existing segment. If blank, it is assumed the turn lane is the depth of the entire length of the represented segment. For block to block representations, this parameter is required, and only works for symmetrical end points of intersections. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This specifies the turn lane depth for the start point of the existing segment. If blank, it is assumed the turn lane is the depth of the entire length of the represented segment. For block to block representations, this parameter is required, and only works for symmetrical end points of intersections. </t>
+  </si>
+  <si>
+    <t>A loading zone; primarily for passenger pickup/drop-off.</t>
+  </si>
+  <si>
+    <t>A zone where commerce is permitted; e.g. food trucks; farmer's markets; newsstands</t>
+  </si>
+  <si>
+    <t>Any slice that has been reconfigured for a temporary purpose; e.g. construction</t>
   </si>
 </sst>
 </file>
@@ -1317,8 +1341,8 @@
   </sheetPr>
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1337,7 +1361,7 @@
     </row>
     <row r="3" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1362,7 +1386,7 @@
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -1379,7 +1403,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>97</v>
+        <v>284</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>9</v>
@@ -1399,7 +1423,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>9</v>
@@ -1419,7 +1443,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>9</v>
@@ -1467,10 +1491,10 @@
     </row>
     <row r="11" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
@@ -1479,10 +1503,10 @@
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1639,10 +1663,10 @@
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -1665,7 +1689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
@@ -1679,10 +1703,10 @@
         <v>15</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>226</v>
+        <v>286</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>227</v>
+        <v>281</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1719,10 +1743,10 @@
         <v>15</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1759,10 +1783,10 @@
         <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -1779,7 +1803,7 @@
         <v>15</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>9</v>
@@ -1799,7 +1823,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>9</v>
@@ -1827,10 +1851,10 @@
     </row>
     <row r="29" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>48</v>
@@ -1839,10 +1863,10 @@
         <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>260</v>
+        <v>283</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -1859,7 +1883,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F30" s="8" t="s">
         <v>9</v>
@@ -1879,7 +1903,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>9</v>
@@ -1899,7 +1923,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>9</v>
@@ -1919,7 +1943,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F33" s="8" t="s">
         <v>9</v>
@@ -1939,7 +1963,7 @@
         <v>15</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>9</v>
@@ -1959,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F35" s="8" t="s">
         <v>9</v>
@@ -1979,7 +2003,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>9</v>
@@ -1999,10 +2023,10 @@
         <v>15</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2019,13 +2043,13 @@
         <v>2</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:6" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2" t="s">
         <v>79</v>
       </c>
@@ -2039,10 +2063,10 @@
         <v>15</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>226</v>
+        <v>282</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>227</v>
+        <v>281</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2059,7 +2083,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>9</v>
@@ -2079,10 +2103,10 @@
         <v>15</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2139,10 +2163,10 @@
         <v>15</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>238</v>
+        <v>287</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
@@ -2159,18 +2183,18 @@
         <v>15</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>238</v>
+        <v>287</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B46" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>6</v>
@@ -2179,7 +2203,7 @@
         <v>15</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>224</v>
+        <v>288</v>
       </c>
       <c r="F46" s="8" t="s">
         <v>9</v>
@@ -2187,10 +2211,10 @@
     </row>
     <row r="47" spans="1:6" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>48</v>
@@ -2199,10 +2223,10 @@
         <v>15</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>237</v>
+        <v>289</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2273,7 +2297,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2324,24 +2348,24 @@
         <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D6" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2392,7 +2416,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2409,15 +2433,15 @@
         <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>112</v>
@@ -2443,7 +2467,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -2458,7 +2482,7 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2479,7 +2503,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2535,7 +2559,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
@@ -2553,7 +2577,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -2607,7 +2631,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -2631,7 +2655,7 @@
     <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -2674,10 +2698,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A69" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2707,7 +2731,7 @@
         <v>120</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -2734,7 +2758,7 @@
     <row r="7" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
@@ -2744,7 +2768,7 @@
         <v>128</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2760,7 +2784,7 @@
         <v>128</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2776,7 +2800,7 @@
         <v>128</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -2792,14 +2816,14 @@
         <v>128</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>106</v>
@@ -2808,14 +2832,14 @@
         <v>128</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>106</v>
@@ -2824,7 +2848,7 @@
         <v>128</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1" ht="29.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2872,7 +2896,7 @@
         <v>135</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -2891,72 +2915,72 @@
     </row>
     <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="D18" t="s">
         <v>130</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="D19" t="s">
         <v>130</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D20" t="s">
         <v>112</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="D21" t="s">
         <v>112</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="D22" t="s">
         <v>112</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -2970,7 +2994,7 @@
         <v>15</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="29.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2986,7 +3010,7 @@
         <v>133</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3077,7 +3101,7 @@
         <v>2</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3105,7 +3129,7 @@
         <v>15</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3138,10 +3162,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3155,12 +3179,12 @@
         <v>15</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="D40" t="s">
         <v>139</v>
@@ -3169,7 +3193,7 @@
         <v>15</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -3194,13 +3218,16 @@
         <v>153</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>167</v>
       </c>
+      <c r="D45" t="s">
+        <v>112</v>
+      </c>
       <c r="E45" s="2" t="s">
         <v>128</v>
       </c>
@@ -3210,7 +3237,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>177</v>
+        <v>277</v>
+      </c>
+      <c r="D46" t="s">
+        <v>112</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>128</v>
@@ -3223,6 +3253,9 @@
       <c r="A47" t="s">
         <v>145</v>
       </c>
+      <c r="D47" t="s">
+        <v>112</v>
+      </c>
       <c r="E47" s="2" t="s">
         <v>128</v>
       </c>
@@ -3232,199 +3265,259 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>171</v>
+        <v>272</v>
+      </c>
+      <c r="D48" t="s">
+        <v>112</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>172</v>
+        <v>171</v>
+      </c>
+      <c r="D49" t="s">
+        <v>112</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>250</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>174</v>
+        <v>279</v>
+      </c>
+      <c r="D50" t="s">
+        <v>112</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>251</v>
+        <v>280</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>278</v>
+      </c>
+      <c r="D51" t="s">
+        <v>112</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>184</v>
+        <v>293</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>179</v>
+        <v>175</v>
+      </c>
+      <c r="D52" t="s">
+        <v>112</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>185</v>
+        <v>176</v>
+      </c>
+      <c r="D53" t="s">
+        <v>112</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="F54" s="2"/>
+      <c r="A54" t="s">
+        <v>182</v>
+      </c>
+      <c r="D54" t="s">
+        <v>112</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="F55" s="2"/>
+      <c r="A55" t="s">
+        <v>273</v>
+      </c>
+      <c r="D55" t="s">
+        <v>112</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
+        <v>275</v>
+      </c>
+      <c r="D56" t="s">
+        <v>112</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
         <v>147</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="F56" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B57" t="s">
+      <c r="F59" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B60" t="s">
         <v>108</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" t="s">
+      <c r="F60" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
         <v>148</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B59" t="s">
+      <c r="F61" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B62" t="s">
         <v>108</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" t="s">
-        <v>149</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B61" t="s">
-        <v>108</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B62" t="s">
-        <v>173</v>
-      </c>
       <c r="F62" s="2" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" t="s">
-        <v>180</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>128</v>
+      <c r="F63" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B64" t="s">
+        <v>108</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B65" t="s">
-        <v>108</v>
+        <v>172</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="F66" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F66" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="7"/>
-      <c r="F68" s="8"/>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68" t="s">
+        <v>108</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" t="s">
+        <v>180</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" t="s">
+        <v>178</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="7"/>
+      <c r="F71" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3456,10 +3549,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3490,7 +3583,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -3504,7 +3597,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -3518,7 +3611,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -3526,7 +3619,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
@@ -3546,7 +3639,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -3560,7 +3653,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -3574,7 +3667,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -3588,7 +3681,7 @@
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -3602,7 +3695,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
@@ -3616,7 +3709,7 @@
         <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -3630,7 +3723,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -3658,7 +3751,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -3686,7 +3779,7 @@
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -3714,7 +3807,7 @@
         <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -3742,7 +3835,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D21" s="2">
         <v>1</v>
@@ -3756,7 +3849,7 @@
         <v>83</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -3770,7 +3863,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
@@ -3778,7 +3871,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>84</v>
@@ -3798,7 +3891,7 @@
         <v>85</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -3812,7 +3905,7 @@
         <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -3826,7 +3919,7 @@
         <v>87</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D27" s="2">
         <v>0</v>
@@ -3840,7 +3933,7 @@
         <v>88</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D28" s="2">
         <v>0</v>
@@ -3854,7 +3947,7 @@
         <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D29" s="2">
         <v>1</v>
@@ -3868,7 +3961,7 @@
         <v>90</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D30" s="2">
         <v>0</v>
@@ -3882,7 +3975,7 @@
         <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D31" s="2">
         <v>0</v>
@@ -3910,7 +4003,7 @@
         <v>93</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -3938,7 +4031,7 @@
         <v>43</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D35" s="2">
         <v>0</v>
@@ -3966,7 +4059,7 @@
         <v>59</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D37" s="2">
         <v>0</v>
@@ -3980,7 +4073,7 @@
         <v>60</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D38" s="2">
         <v>0</v>
@@ -4016,13 +4109,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B41" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
@@ -4030,10 +4123,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B42" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>48</v>

</xml_diff>